<commit_message>
Updates GOOG, TSLA and other
</commit_message>
<xml_diff>
--- a/TSLA.xlsx
+++ b/TSLA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.Finance\Anaylsen\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77821B26-A675-45EF-8BD3-261E3708DCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4452826-844E-4CD9-B3F8-9CBD314CD29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="4680" windowWidth="38175" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -752,7 +752,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -808,6 +807,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -833,13 +833,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>10117</xdr:colOff>
+      <xdr:colOff>551851</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>25572</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>7712</xdr:colOff>
       <xdr:row>136</xdr:row>
       <xdr:rowOff>117330</xdr:rowOff>
     </xdr:to>
@@ -858,7 +858,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19679242" y="47625"/>
+          <a:off x="20220976" y="47625"/>
           <a:ext cx="15455" cy="21929580"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -885,15 +885,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>21322</xdr:colOff>
+      <xdr:colOff>705932</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>21322</xdr:colOff>
+      <xdr:colOff>705932</xdr:colOff>
       <xdr:row>127</xdr:row>
-      <xdr:rowOff>20053</xdr:rowOff>
+      <xdr:rowOff>43865</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -908,8 +908,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28857006" y="0"/>
-          <a:ext cx="0" cy="19591421"/>
+          <a:off x="29465479" y="23812"/>
+          <a:ext cx="0" cy="20433319"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1248,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="E1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1259,32 +1259,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>108</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="11">
-        <v>254.5</v>
+      <c r="K2" s="42">
+        <v>312.19</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>124</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="10">
-        <v>3220.9562110000002</v>
-      </c>
-      <c r="L3" s="42" t="s">
-        <v>120</v>
+        <v>3225.4488889999998</v>
+      </c>
+      <c r="L3" s="41" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="32" t="s">
         <v>125</v>
       </c>
       <c r="J4" s="9" t="s">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="K4" s="10">
         <f>K2*K3</f>
-        <v>819733.35569950007</v>
+        <v>1006952.8886569099</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
@@ -1300,30 +1300,30 @@
         <v>3</v>
       </c>
       <c r="K5" s="10">
-        <f>16352+20644</f>
-        <v>36996</v>
-      </c>
-      <c r="L5" s="42" t="s">
-        <v>120</v>
+        <f>15587+21195</f>
+        <v>36782</v>
+      </c>
+      <c r="L5" s="41" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="32" t="s">
         <v>156</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="18">
-        <f>5292+2237</f>
-        <v>7529</v>
-      </c>
-      <c r="L6" s="42" t="s">
-        <v>120</v>
+      <c r="K6" s="17">
+        <f>2040+5180</f>
+        <v>7220</v>
+      </c>
+      <c r="L6" s="41" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="32" t="s">
         <v>155</v>
       </c>
       <c r="J7" s="9" t="s">
@@ -1331,30 +1331,31 @@
       </c>
       <c r="K7" s="10">
         <f>K4-K5+K6</f>
-        <v>790266.35569950007</v>
+        <v>977390.88865690993</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="32" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="J9" s="33" t="s">
+      <c r="D9" s="32"/>
+      <c r="J9" s="32" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="J10" s="33" t="s">
+      <c r="J10" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="K10" s="33" t="s">
+      <c r="K10" s="32" t="s">
         <v>169</v>
       </c>
     </row>
@@ -1364,7 +1365,7 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="32" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1382,11 +1383,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E310252-7C49-48D8-9A64-7380C8DB275B}">
   <dimension ref="A1:DE123"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AD54" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="Z3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE91" sqref="AE91"/>
+      <selection pane="bottomRight" activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1408,22 +1409,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="C2" s="27" t="s">
+      <c r="A2" s="13"/>
+      <c r="C2" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="26" t="s">
         <v>96</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1474,40 +1475,40 @@
       <c r="V2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="W2" s="16" t="s">
+      <c r="W2" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="X2" s="16" t="s">
+      <c r="X2" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="Y2" s="16" t="s">
+      <c r="Y2" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="Z2" s="16" t="s">
+      <c r="Z2" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="AA2" s="27" t="s">
+      <c r="AA2" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="AB2" s="27" t="s">
+      <c r="AB2" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="AC2" s="27" t="s">
+      <c r="AC2" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="AD2" s="27" t="s">
+      <c r="AD2" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="AE2" s="31" t="s">
+      <c r="AE2" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="AF2" s="31" t="s">
+      <c r="AF2" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="AG2" s="31" t="s">
+      <c r="AG2" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="AH2" s="31" t="s">
+      <c r="AH2" s="30" t="s">
         <v>123</v>
       </c>
       <c r="AJ2" s="1">
@@ -1596,168 +1597,168 @@
       </c>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="33" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="W3" s="16"/>
-      <c r="X3" s="16"/>
-      <c r="Y3" s="16"/>
-      <c r="Z3" s="16"/>
-      <c r="AA3" s="36">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="35">
         <f>158800/2*1.12</f>
         <v>88928.000000000015</v>
       </c>
-      <c r="AB3" s="36">
+      <c r="AB3" s="35">
         <f>158800/2*1.12</f>
         <v>88928.000000000015</v>
       </c>
-      <c r="AC3" s="27"/>
-      <c r="AD3" s="27"/>
-      <c r="AE3" s="31"/>
-      <c r="AF3" s="31"/>
-      <c r="AG3" s="31"/>
-      <c r="AH3" s="31"/>
+      <c r="AC3" s="26"/>
+      <c r="AD3" s="26"/>
+      <c r="AE3" s="30"/>
+      <c r="AF3" s="30"/>
+      <c r="AG3" s="30"/>
+      <c r="AH3" s="30"/>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="33" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="36">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="35">
         <f>10845224/145</f>
         <v>74794.64827586207</v>
       </c>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="31"/>
-      <c r="AF4" s="31"/>
-      <c r="AG4" s="31"/>
-      <c r="AH4" s="31"/>
+      <c r="AC4" s="26"/>
+      <c r="AD4" s="26"/>
+      <c r="AE4" s="30"/>
+      <c r="AF4" s="30"/>
+      <c r="AG4" s="30"/>
+      <c r="AH4" s="30"/>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="33" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="W5" s="16"/>
-      <c r="X5" s="36">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="35">
         <v>41254</v>
       </c>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="27"/>
-      <c r="AB5" s="36">
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="35">
         <v>44060</v>
       </c>
-      <c r="AC5" s="27"/>
-      <c r="AD5" s="27"/>
-      <c r="AE5" s="31"/>
-      <c r="AF5" s="31"/>
-      <c r="AG5" s="31"/>
-      <c r="AH5" s="31"/>
+      <c r="AC5" s="26"/>
+      <c r="AD5" s="26"/>
+      <c r="AE5" s="30"/>
+      <c r="AF5" s="30"/>
+      <c r="AG5" s="30"/>
+      <c r="AH5" s="30"/>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="33" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="36">
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="35">
         <v>44811</v>
       </c>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="27"/>
-      <c r="AB6" s="36">
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="35">
         <v>42427</v>
       </c>
-      <c r="AC6" s="27"/>
-      <c r="AD6" s="27"/>
-      <c r="AE6" s="31"/>
-      <c r="AF6" s="31"/>
-      <c r="AG6" s="31"/>
-      <c r="AH6" s="31"/>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="26"/>
+      <c r="AE6" s="30"/>
+      <c r="AF6" s="30"/>
+      <c r="AG6" s="30"/>
+      <c r="AH6" s="30"/>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="33" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="36"/>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="35">
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="35"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="34">
         <f>63009-AB7</f>
         <v>30939</v>
       </c>
-      <c r="AB7" s="36">
+      <c r="AB7" s="35">
         <v>32070</v>
       </c>
-      <c r="AC7" s="27"/>
-      <c r="AD7" s="27"/>
-      <c r="AE7" s="31"/>
-      <c r="AF7" s="31"/>
-      <c r="AG7" s="31"/>
-      <c r="AH7" s="31"/>
+      <c r="AC7" s="26"/>
+      <c r="AD7" s="26"/>
+      <c r="AE7" s="30"/>
+      <c r="AF7" s="30"/>
+      <c r="AG7" s="30"/>
+      <c r="AH7" s="30"/>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="33" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="W8" s="36"/>
-      <c r="X8" s="36">
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="35">
         <f>28244*1.12</f>
         <v>31633.280000000002</v>
       </c>
-      <c r="Y8" s="16"/>
-      <c r="Z8" s="16"/>
-      <c r="AA8" s="27"/>
-      <c r="AB8" s="36">
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="26"/>
+      <c r="AB8" s="35">
         <f>27710*1.12</f>
         <v>31035.200000000004</v>
       </c>
-      <c r="AC8" s="27"/>
-      <c r="AD8" s="27"/>
-      <c r="AE8" s="31"/>
-      <c r="AF8" s="31"/>
-      <c r="AG8" s="31"/>
-      <c r="AH8" s="31"/>
-    </row>
-    <row r="9" spans="1:58" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="38"/>
-      <c r="B9" s="23" t="s">
+      <c r="AC8" s="26"/>
+      <c r="AD8" s="26"/>
+      <c r="AE8" s="30"/>
+      <c r="AF8" s="30"/>
+      <c r="AG8" s="30"/>
+      <c r="AH8" s="30"/>
+    </row>
+    <row r="9" spans="1:58" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="37"/>
+      <c r="B9" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C9" s="7">
@@ -1864,12 +1865,12 @@
         <f t="shared" si="8"/>
         <v>18530</v>
       </c>
-      <c r="AC9" s="24"/>
-      <c r="AD9" s="24"/>
-      <c r="AE9" s="24"/>
-      <c r="AF9" s="24"/>
-      <c r="AG9" s="24"/>
-      <c r="AH9" s="24"/>
+      <c r="AC9" s="23"/>
+      <c r="AD9" s="23"/>
+      <c r="AE9" s="23"/>
+      <c r="AF9" s="23"/>
+      <c r="AG9" s="23"/>
+      <c r="AH9" s="23"/>
       <c r="AO9" s="6">
         <f t="shared" ref="AO9:AU9" si="9">+AO45</f>
         <v>0</v>
@@ -1900,303 +1901,303 @@
       </c>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="33" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="W10" s="16"/>
-      <c r="X10" s="16"/>
-      <c r="Y10" s="16"/>
-      <c r="Z10" s="16"/>
-      <c r="AA10" s="35">
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+      <c r="AA10" s="34">
         <v>16300</v>
       </c>
-      <c r="AB10" s="35">
+      <c r="AB10" s="34">
         <f>(228316.903/7)-AA10</f>
         <v>16316.700428571428</v>
       </c>
-      <c r="AC10" s="27"/>
-      <c r="AD10" s="27"/>
-      <c r="AE10" s="31"/>
-      <c r="AF10" s="31"/>
-      <c r="AG10" s="31"/>
-      <c r="AH10" s="31"/>
+      <c r="AC10" s="26"/>
+      <c r="AD10" s="26"/>
+      <c r="AE10" s="30"/>
+      <c r="AF10" s="30"/>
+      <c r="AG10" s="30"/>
+      <c r="AH10" s="30"/>
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="33" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="37"/>
-      <c r="Y11" s="37"/>
-      <c r="Z11" s="37"/>
-      <c r="AA11" s="36">
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="36"/>
+      <c r="Y11" s="36"/>
+      <c r="Z11" s="36"/>
+      <c r="AA11" s="35">
         <f>9728.5/1.12</f>
         <v>8686.1607142857138</v>
       </c>
-      <c r="AB11" s="35">
+      <c r="AB11" s="34">
         <f>9728.5/1.12</f>
         <v>8686.1607142857138</v>
       </c>
-      <c r="AC11" s="27"/>
-      <c r="AD11" s="27"/>
-      <c r="AE11" s="31"/>
-      <c r="AF11" s="31"/>
-      <c r="AG11" s="31"/>
-      <c r="AH11" s="31"/>
+      <c r="AC11" s="26"/>
+      <c r="AD11" s="26"/>
+      <c r="AE11" s="30"/>
+      <c r="AF11" s="30"/>
+      <c r="AG11" s="30"/>
+      <c r="AH11" s="30"/>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="37"/>
-      <c r="Y12" s="37"/>
-      <c r="Z12" s="37"/>
-      <c r="AA12" s="36"/>
-      <c r="AB12" s="35"/>
-      <c r="AC12" s="27"/>
-      <c r="AD12" s="27"/>
-      <c r="AE12" s="31"/>
-      <c r="AF12" s="31"/>
-      <c r="AG12" s="31"/>
-      <c r="AH12" s="31"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="36"/>
+      <c r="Y12" s="36"/>
+      <c r="Z12" s="36"/>
+      <c r="AA12" s="35"/>
+      <c r="AB12" s="34"/>
+      <c r="AC12" s="26"/>
+      <c r="AD12" s="26"/>
+      <c r="AE12" s="30"/>
+      <c r="AF12" s="30"/>
+      <c r="AG12" s="30"/>
+      <c r="AH12" s="30"/>
     </row>
     <row r="13" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="33" t="s">
+      <c r="A13" s="13"/>
+      <c r="B13" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="W13" s="16"/>
-      <c r="X13" s="16"/>
-      <c r="Y13" s="16"/>
-      <c r="Z13" s="16"/>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="36">
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="26"/>
+      <c r="AB13" s="35">
         <v>2186000</v>
       </c>
-      <c r="AC13" s="27"/>
-      <c r="AD13" s="27"/>
-      <c r="AE13" s="31"/>
-      <c r="AF13" s="31"/>
-      <c r="AG13" s="31"/>
-      <c r="AH13" s="31"/>
+      <c r="AC13" s="26"/>
+      <c r="AD13" s="26"/>
+      <c r="AE13" s="30"/>
+      <c r="AF13" s="30"/>
+      <c r="AG13" s="30"/>
+      <c r="AH13" s="30"/>
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="33" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="W14" s="37">
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="W14" s="36">
         <f>4372000-X14</f>
         <v>2041000</v>
       </c>
-      <c r="X14" s="37">
+      <c r="X14" s="36">
         <v>2331000</v>
       </c>
-      <c r="Y14" s="37"/>
-      <c r="Z14" s="37"/>
-      <c r="AA14" s="35">
+      <c r="Y14" s="36"/>
+      <c r="Z14" s="36"/>
+      <c r="AA14" s="34">
         <f>4348000-AB14</f>
         <v>2104000</v>
       </c>
-      <c r="AB14" s="36">
+      <c r="AB14" s="35">
         <v>2244000</v>
       </c>
-      <c r="AC14" s="27"/>
-      <c r="AD14" s="27"/>
-      <c r="AE14" s="31"/>
-      <c r="AF14" s="31"/>
-      <c r="AG14" s="31"/>
-      <c r="AH14" s="31"/>
+      <c r="AC14" s="26"/>
+      <c r="AD14" s="26"/>
+      <c r="AE14" s="30"/>
+      <c r="AF14" s="30"/>
+      <c r="AG14" s="30"/>
+      <c r="AH14" s="30"/>
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="33" t="s">
+      <c r="A15" s="13"/>
+      <c r="B15" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="W15" s="37"/>
-      <c r="X15" s="37"/>
-      <c r="Y15" s="37"/>
-      <c r="Z15" s="37"/>
-      <c r="AA15" s="35"/>
-      <c r="AB15" s="35">
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="W15" s="36"/>
+      <c r="X15" s="36"/>
+      <c r="Y15" s="36"/>
+      <c r="Z15" s="36"/>
+      <c r="AA15" s="34"/>
+      <c r="AB15" s="34">
         <f>375000+26000+741000</f>
         <v>1142000</v>
       </c>
-      <c r="AC15" s="27"/>
-      <c r="AD15" s="27"/>
-      <c r="AE15" s="31"/>
-      <c r="AF15" s="31"/>
-      <c r="AG15" s="31"/>
-      <c r="AH15" s="31"/>
+      <c r="AC15" s="26"/>
+      <c r="AD15" s="26"/>
+      <c r="AE15" s="30"/>
+      <c r="AF15" s="30"/>
+      <c r="AG15" s="30"/>
+      <c r="AH15" s="30"/>
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="33" t="s">
+      <c r="A16" s="13"/>
+      <c r="B16" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="W16" s="37">
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="W16" s="36">
         <f>1844000-X16</f>
         <v>865000</v>
       </c>
-      <c r="X16" s="36">
+      <c r="X16" s="35">
         <v>979000</v>
       </c>
-      <c r="Y16" s="37"/>
-      <c r="Z16" s="37"/>
-      <c r="AA16" s="35">
+      <c r="Y16" s="36"/>
+      <c r="Z16" s="36"/>
+      <c r="AA16" s="34">
         <f>1938000-AB16</f>
         <v>895000</v>
       </c>
-      <c r="AB16" s="36">
+      <c r="AB16" s="35">
         <v>1043000</v>
       </c>
-      <c r="AC16" s="27"/>
-      <c r="AD16" s="27"/>
-      <c r="AE16" s="31"/>
-      <c r="AF16" s="31"/>
-      <c r="AG16" s="31"/>
-      <c r="AH16" s="31"/>
+      <c r="AC16" s="26"/>
+      <c r="AD16" s="26"/>
+      <c r="AE16" s="30"/>
+      <c r="AF16" s="30"/>
+      <c r="AG16" s="30"/>
+      <c r="AH16" s="30"/>
     </row>
     <row r="17" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="33" t="s">
+      <c r="A17" s="13"/>
+      <c r="B17" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="W17" s="16"/>
-      <c r="X17" s="37">
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="36">
         <f>252657+246259+209448</f>
         <v>708364</v>
       </c>
-      <c r="Y17" s="37"/>
-      <c r="Z17" s="37"/>
-      <c r="AA17" s="35"/>
-      <c r="AB17" s="35">
+      <c r="Y17" s="36"/>
+      <c r="Z17" s="36"/>
+      <c r="AA17" s="34"/>
+      <c r="AB17" s="34">
         <f>341671+344008+334039</f>
         <v>1019718</v>
       </c>
-      <c r="AC17" s="27"/>
-      <c r="AD17" s="27"/>
-      <c r="AE17" s="31"/>
-      <c r="AF17" s="31"/>
-      <c r="AG17" s="31"/>
-      <c r="AH17" s="31"/>
+      <c r="AC17" s="26"/>
+      <c r="AD17" s="26"/>
+      <c r="AE17" s="30"/>
+      <c r="AF17" s="30"/>
+      <c r="AG17" s="30"/>
+      <c r="AH17" s="30"/>
     </row>
     <row r="18" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="33" t="s">
+      <c r="A18" s="13"/>
+      <c r="B18" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="W18" s="37">
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="W18" s="36">
         <f>1214864-X18</f>
         <v>588138</v>
       </c>
-      <c r="X18" s="37">
+      <c r="X18" s="36">
         <v>626726</v>
       </c>
-      <c r="Y18" s="37"/>
-      <c r="Z18" s="37"/>
-      <c r="AA18" s="35">
+      <c r="Y18" s="36"/>
+      <c r="Z18" s="36"/>
+      <c r="AA18" s="34">
         <f>1213276-AB18</f>
         <v>594533</v>
       </c>
-      <c r="AB18" s="35">
+      <c r="AB18" s="34">
         <v>618743</v>
       </c>
-      <c r="AC18" s="27"/>
-      <c r="AD18" s="27"/>
-      <c r="AE18" s="31"/>
-      <c r="AF18" s="31"/>
-      <c r="AG18" s="31"/>
-      <c r="AH18" s="31"/>
+      <c r="AC18" s="26"/>
+      <c r="AD18" s="26"/>
+      <c r="AE18" s="30"/>
+      <c r="AF18" s="30"/>
+      <c r="AG18" s="30"/>
+      <c r="AH18" s="30"/>
     </row>
     <row r="19" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="33" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="W19" s="16"/>
-      <c r="X19" s="37">
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="36">
         <v>515746</v>
       </c>
-      <c r="Y19" s="37"/>
-      <c r="Z19" s="37"/>
-      <c r="AA19" s="35"/>
-      <c r="AB19" s="35">
+      <c r="Y19" s="36"/>
+      <c r="Z19" s="36"/>
+      <c r="AA19" s="34"/>
+      <c r="AB19" s="34">
         <v>496712</v>
       </c>
-      <c r="AC19" s="27"/>
-      <c r="AD19" s="27"/>
-      <c r="AE19" s="31"/>
-      <c r="AF19" s="31"/>
-      <c r="AG19" s="31"/>
-      <c r="AH19" s="31"/>
-    </row>
-    <row r="20" spans="1:47" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="38"/>
-      <c r="B20" s="23" t="s">
+      <c r="AC19" s="26"/>
+      <c r="AD19" s="26"/>
+      <c r="AE19" s="30"/>
+      <c r="AF19" s="30"/>
+      <c r="AG19" s="30"/>
+      <c r="AH19" s="30"/>
+    </row>
+    <row r="20" spans="1:47" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="37"/>
+      <c r="B20" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24"/>
-      <c r="U20" s="24"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="23"/>
       <c r="V20" s="7">
         <f t="shared" ref="V20:AA20" si="10">+V42</f>
         <v>439701</v>
@@ -2225,12 +2226,12 @@
         <f>+AB42</f>
         <v>410831</v>
       </c>
-      <c r="AC20" s="24"/>
-      <c r="AD20" s="24"/>
-      <c r="AE20" s="24"/>
-      <c r="AF20" s="24"/>
-      <c r="AG20" s="24"/>
-      <c r="AH20" s="24"/>
+      <c r="AC20" s="23"/>
+      <c r="AD20" s="23"/>
+      <c r="AE20" s="23"/>
+      <c r="AF20" s="23"/>
+      <c r="AG20" s="23"/>
+      <c r="AH20" s="23"/>
       <c r="AT20" s="6">
         <f>+AT37</f>
         <v>1808581</v>
@@ -2241,322 +2242,322 @@
       </c>
     </row>
     <row r="21" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="33" t="s">
+      <c r="A21" s="13"/>
+      <c r="B21" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="W21" s="16"/>
-      <c r="X21" s="37"/>
-      <c r="Y21" s="37"/>
-      <c r="Z21" s="37"/>
-      <c r="AA21" s="36">
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="36"/>
+      <c r="Y21" s="36"/>
+      <c r="Z21" s="36"/>
+      <c r="AA21" s="35">
         <f>+AB21</f>
         <v>77972.5</v>
       </c>
-      <c r="AB21" s="35">
+      <c r="AB21" s="34">
         <f>155945/2</f>
         <v>77972.5</v>
       </c>
-      <c r="AC21" s="27"/>
-      <c r="AD21" s="27"/>
-      <c r="AE21" s="31"/>
-      <c r="AF21" s="31"/>
-      <c r="AG21" s="31"/>
-      <c r="AH21" s="31"/>
+      <c r="AC21" s="26"/>
+      <c r="AD21" s="26"/>
+      <c r="AE21" s="30"/>
+      <c r="AF21" s="30"/>
+      <c r="AG21" s="30"/>
+      <c r="AH21" s="30"/>
     </row>
     <row r="22" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="W22" s="16"/>
-      <c r="X22" s="37"/>
-      <c r="Y22" s="37"/>
-      <c r="Z22" s="37"/>
-      <c r="AA22" s="36"/>
-      <c r="AB22" s="35"/>
-      <c r="AC22" s="27"/>
-      <c r="AD22" s="27"/>
-      <c r="AE22" s="31"/>
-      <c r="AF22" s="31"/>
-      <c r="AG22" s="31"/>
-      <c r="AH22" s="31"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="36"/>
+      <c r="Y22" s="36"/>
+      <c r="Z22" s="36"/>
+      <c r="AA22" s="35"/>
+      <c r="AB22" s="34"/>
+      <c r="AC22" s="26"/>
+      <c r="AD22" s="26"/>
+      <c r="AE22" s="30"/>
+      <c r="AF22" s="30"/>
+      <c r="AG22" s="30"/>
+      <c r="AH22" s="30"/>
     </row>
     <row r="23" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="33" t="s">
+      <c r="A23" s="13"/>
+      <c r="B23" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="W23" s="16"/>
-      <c r="X23" s="37"/>
-      <c r="Y23" s="37"/>
-      <c r="Z23" s="37"/>
-      <c r="AA23" s="36"/>
-      <c r="AB23" s="35">
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="36"/>
+      <c r="Y23" s="36"/>
+      <c r="Z23" s="36"/>
+      <c r="AA23" s="35"/>
+      <c r="AB23" s="34">
         <f>+AB4*1000000/AB13</f>
         <v>34215.301132599299</v>
       </c>
-      <c r="AC23" s="27"/>
-      <c r="AD23" s="27"/>
-      <c r="AE23" s="31"/>
-      <c r="AF23" s="31"/>
-      <c r="AG23" s="31"/>
-      <c r="AH23" s="31"/>
+      <c r="AC23" s="26"/>
+      <c r="AD23" s="26"/>
+      <c r="AE23" s="30"/>
+      <c r="AF23" s="30"/>
+      <c r="AG23" s="30"/>
+      <c r="AH23" s="30"/>
     </row>
     <row r="24" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="33" t="s">
+      <c r="A24" s="13"/>
+      <c r="B24" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="W24" s="16"/>
-      <c r="X24" s="37"/>
-      <c r="Y24" s="37"/>
-      <c r="Z24" s="37"/>
-      <c r="AA24" s="36"/>
-      <c r="AB24" s="36">
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="W24" s="15"/>
+      <c r="X24" s="36"/>
+      <c r="Y24" s="36"/>
+      <c r="Z24" s="36"/>
+      <c r="AA24" s="35"/>
+      <c r="AB24" s="35">
         <f>+AB3*1000000/AB14</f>
         <v>39629.233511586463</v>
       </c>
-      <c r="AC24" s="27"/>
-      <c r="AD24" s="27"/>
-      <c r="AE24" s="31"/>
-      <c r="AF24" s="31"/>
-      <c r="AG24" s="31"/>
-      <c r="AH24" s="31"/>
+      <c r="AC24" s="26"/>
+      <c r="AD24" s="26"/>
+      <c r="AE24" s="30"/>
+      <c r="AF24" s="30"/>
+      <c r="AG24" s="30"/>
+      <c r="AH24" s="30"/>
     </row>
     <row r="25" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
-      <c r="B25" s="33" t="s">
+      <c r="A25" s="13"/>
+      <c r="B25" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="W25" s="16"/>
-      <c r="X25" s="37"/>
-      <c r="Y25" s="37"/>
-      <c r="Z25" s="37"/>
-      <c r="AA25" s="36"/>
-      <c r="AB25" s="35">
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="W25" s="15"/>
+      <c r="X25" s="36"/>
+      <c r="Y25" s="36"/>
+      <c r="Z25" s="36"/>
+      <c r="AA25" s="35"/>
+      <c r="AB25" s="34">
         <f>+AB5*1000000/AB16</f>
         <v>42243.528283796739</v>
       </c>
-      <c r="AC25" s="27"/>
-      <c r="AD25" s="27"/>
-      <c r="AE25" s="31"/>
-      <c r="AF25" s="31"/>
-      <c r="AG25" s="31"/>
-      <c r="AH25" s="31"/>
+      <c r="AC25" s="26"/>
+      <c r="AD25" s="26"/>
+      <c r="AE25" s="30"/>
+      <c r="AF25" s="30"/>
+      <c r="AG25" s="30"/>
+      <c r="AH25" s="30"/>
     </row>
     <row r="26" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="33" t="s">
+      <c r="A26" s="13"/>
+      <c r="B26" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="W26" s="16"/>
-      <c r="X26" s="37"/>
-      <c r="Y26" s="37"/>
-      <c r="Z26" s="37"/>
-      <c r="AA26" s="36"/>
-      <c r="AB26" s="35">
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="W26" s="15"/>
+      <c r="X26" s="36"/>
+      <c r="Y26" s="36"/>
+      <c r="Z26" s="36"/>
+      <c r="AA26" s="35"/>
+      <c r="AB26" s="34">
         <f>+AB6*1000000/AB15</f>
         <v>37151.488616462346</v>
       </c>
-      <c r="AC26" s="27"/>
-      <c r="AD26" s="27"/>
-      <c r="AE26" s="31"/>
-      <c r="AF26" s="31"/>
-      <c r="AG26" s="31"/>
-      <c r="AH26" s="31"/>
+      <c r="AC26" s="26"/>
+      <c r="AD26" s="26"/>
+      <c r="AE26" s="30"/>
+      <c r="AF26" s="30"/>
+      <c r="AG26" s="30"/>
+      <c r="AH26" s="30"/>
     </row>
     <row r="27" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="33" t="s">
+      <c r="A27" s="13"/>
+      <c r="B27" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="W27" s="16"/>
-      <c r="X27" s="37"/>
-      <c r="Y27" s="37"/>
-      <c r="Z27" s="37"/>
-      <c r="AA27" s="36"/>
-      <c r="AB27" s="35">
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="W27" s="15"/>
+      <c r="X27" s="36"/>
+      <c r="Y27" s="36"/>
+      <c r="Z27" s="36"/>
+      <c r="AA27" s="35"/>
+      <c r="AB27" s="34">
         <f>+AB10*1000000/AB17</f>
         <v>16001.188984181341</v>
       </c>
-      <c r="AC27" s="27"/>
-      <c r="AD27" s="27"/>
-      <c r="AE27" s="31"/>
-      <c r="AF27" s="31"/>
-      <c r="AG27" s="31"/>
-      <c r="AH27" s="31"/>
+      <c r="AC27" s="26"/>
+      <c r="AD27" s="26"/>
+      <c r="AE27" s="30"/>
+      <c r="AF27" s="30"/>
+      <c r="AG27" s="30"/>
+      <c r="AH27" s="30"/>
     </row>
     <row r="28" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="33" t="s">
+      <c r="A28" s="13"/>
+      <c r="B28" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="W28" s="16"/>
-      <c r="X28" s="37"/>
-      <c r="Y28" s="37"/>
-      <c r="Z28" s="37"/>
-      <c r="AA28" s="36"/>
-      <c r="AB28" s="35">
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="W28" s="15"/>
+      <c r="X28" s="36"/>
+      <c r="Y28" s="36"/>
+      <c r="Z28" s="36"/>
+      <c r="AA28" s="35"/>
+      <c r="AB28" s="34">
         <f>+AB7*1000000/AB18</f>
         <v>51830.889399960892</v>
       </c>
-      <c r="AC28" s="27"/>
-      <c r="AD28" s="27"/>
-      <c r="AE28" s="31"/>
-      <c r="AF28" s="31"/>
-      <c r="AG28" s="31"/>
-      <c r="AH28" s="31"/>
+      <c r="AC28" s="26"/>
+      <c r="AD28" s="26"/>
+      <c r="AE28" s="30"/>
+      <c r="AF28" s="30"/>
+      <c r="AG28" s="30"/>
+      <c r="AH28" s="30"/>
     </row>
     <row r="29" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="33" t="s">
+      <c r="A29" s="13"/>
+      <c r="B29" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="W29" s="16"/>
-      <c r="X29" s="37"/>
-      <c r="Y29" s="37"/>
-      <c r="Z29" s="37"/>
-      <c r="AA29" s="36"/>
-      <c r="AB29" s="35">
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="W29" s="15"/>
+      <c r="X29" s="36"/>
+      <c r="Y29" s="36"/>
+      <c r="Z29" s="36"/>
+      <c r="AA29" s="35"/>
+      <c r="AB29" s="34">
         <f>+AB8*1000000/AB19</f>
         <v>62481.27687674146</v>
       </c>
-      <c r="AC29" s="27"/>
-      <c r="AD29" s="27"/>
-      <c r="AE29" s="31"/>
-      <c r="AF29" s="31"/>
-      <c r="AG29" s="31"/>
-      <c r="AH29" s="31"/>
+      <c r="AC29" s="26"/>
+      <c r="AD29" s="26"/>
+      <c r="AE29" s="30"/>
+      <c r="AF29" s="30"/>
+      <c r="AG29" s="30"/>
+      <c r="AH29" s="30"/>
     </row>
     <row r="30" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="33" t="s">
+      <c r="A30" s="13"/>
+      <c r="B30" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="W30" s="16"/>
-      <c r="X30" s="37"/>
-      <c r="Y30" s="37"/>
-      <c r="Z30" s="37"/>
-      <c r="AA30" s="36"/>
-      <c r="AB30" s="35">
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="W30" s="15"/>
+      <c r="X30" s="36"/>
+      <c r="Y30" s="36"/>
+      <c r="Z30" s="36"/>
+      <c r="AA30" s="35"/>
+      <c r="AB30" s="34">
         <f>+AB9*1000000/AB20</f>
         <v>45103.704442946124</v>
       </c>
-      <c r="AC30" s="27"/>
-      <c r="AD30" s="27"/>
-      <c r="AE30" s="31"/>
-      <c r="AF30" s="31"/>
-      <c r="AG30" s="31"/>
-      <c r="AH30" s="31"/>
+      <c r="AC30" s="26"/>
+      <c r="AD30" s="26"/>
+      <c r="AE30" s="30"/>
+      <c r="AF30" s="30"/>
+      <c r="AG30" s="30"/>
+      <c r="AH30" s="30"/>
     </row>
     <row r="31" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
-      <c r="B31" s="33" t="s">
+      <c r="A31" s="13"/>
+      <c r="B31" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="W31" s="16"/>
-      <c r="X31" s="37"/>
-      <c r="Y31" s="37"/>
-      <c r="Z31" s="37"/>
-      <c r="AA31" s="36"/>
-      <c r="AB31" s="35">
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="W31" s="15"/>
+      <c r="X31" s="36"/>
+      <c r="Y31" s="36"/>
+      <c r="Z31" s="36"/>
+      <c r="AA31" s="35"/>
+      <c r="AB31" s="34">
         <f>+AB11*1000000/AB21</f>
         <v>111400.31054904887</v>
       </c>
-      <c r="AC31" s="27"/>
-      <c r="AD31" s="27"/>
-      <c r="AE31" s="31"/>
-      <c r="AF31" s="31"/>
-      <c r="AG31" s="31"/>
-      <c r="AH31" s="31"/>
+      <c r="AC31" s="26"/>
+      <c r="AD31" s="26"/>
+      <c r="AE31" s="30"/>
+      <c r="AF31" s="30"/>
+      <c r="AG31" s="30"/>
+      <c r="AH31" s="30"/>
     </row>
     <row r="32" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A32" s="14"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="W32" s="16"/>
-      <c r="X32" s="37"/>
-      <c r="Y32" s="37"/>
-      <c r="Z32" s="37"/>
-      <c r="AA32" s="36"/>
-      <c r="AB32" s="35"/>
-      <c r="AC32" s="27"/>
-      <c r="AD32" s="27"/>
-      <c r="AE32" s="31"/>
-      <c r="AF32" s="31"/>
-      <c r="AG32" s="31"/>
-      <c r="AH32" s="31"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="W32" s="15"/>
+      <c r="X32" s="36"/>
+      <c r="Y32" s="36"/>
+      <c r="Z32" s="36"/>
+      <c r="AA32" s="35"/>
+      <c r="AB32" s="34"/>
+      <c r="AC32" s="26"/>
+      <c r="AD32" s="26"/>
+      <c r="AE32" s="30"/>
+      <c r="AF32" s="30"/>
+      <c r="AG32" s="30"/>
+      <c r="AH32" s="30"/>
     </row>
     <row r="33" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A33" s="14"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="W33" s="16"/>
-      <c r="X33" s="16"/>
-      <c r="Y33" s="16"/>
-      <c r="Z33" s="16"/>
-      <c r="AA33" s="27"/>
-      <c r="AC33" s="27"/>
-      <c r="AD33" s="27"/>
-      <c r="AE33" s="31"/>
-      <c r="AF33" s="31"/>
-      <c r="AG33" s="31"/>
-      <c r="AH33" s="31"/>
+      <c r="A33" s="13"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="W33" s="15"/>
+      <c r="X33" s="15"/>
+      <c r="Y33" s="15"/>
+      <c r="Z33" s="15"/>
+      <c r="AA33" s="26"/>
+      <c r="AC33" s="26"/>
+      <c r="AD33" s="26"/>
+      <c r="AE33" s="30"/>
+      <c r="AF33" s="30"/>
+      <c r="AG33" s="30"/>
+      <c r="AH33" s="30"/>
       <c r="AU33" s="1">
         <f>+AU37*8/1000</f>
         <v>14787.533599999999</v>
       </c>
     </row>
     <row r="34" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C34" s="5"/>
@@ -2676,8 +2677,12 @@
         <f>+Z35*1.3</f>
         <v>29859.7</v>
       </c>
-      <c r="AE35" s="5"/>
-      <c r="AF35" s="5"/>
+      <c r="AE35" s="5">
+        <v>12881</v>
+      </c>
+      <c r="AF35" s="5">
+        <v>10394</v>
+      </c>
       <c r="AG35" s="5"/>
       <c r="AH35" s="5"/>
       <c r="AP35" s="4">
@@ -2787,8 +2792,12 @@
         <f>+Z36*1.1</f>
         <v>507691.80000000005</v>
       </c>
-      <c r="AE36" s="5"/>
-      <c r="AF36" s="5"/>
+      <c r="AE36" s="5">
+        <v>323800</v>
+      </c>
+      <c r="AF36" s="5">
+        <v>373728</v>
+      </c>
       <c r="AG36" s="5"/>
       <c r="AH36" s="5"/>
       <c r="AP36" s="4">
@@ -2873,7 +2882,7 @@
         <v>308600</v>
       </c>
       <c r="S37" s="7">
-        <f t="shared" ref="S37:AD37" si="12">S36+S35</f>
+        <f t="shared" ref="S37:AF37" si="12">S36+S35</f>
         <v>310048</v>
       </c>
       <c r="T37" s="7">
@@ -2920,8 +2929,14 @@
         <f t="shared" si="12"/>
         <v>537551.5</v>
       </c>
-      <c r="AE37" s="7"/>
-      <c r="AF37" s="7"/>
+      <c r="AE37" s="7">
+        <f t="shared" si="12"/>
+        <v>336681</v>
+      </c>
+      <c r="AF37" s="7">
+        <f t="shared" si="12"/>
+        <v>384122</v>
+      </c>
       <c r="AG37" s="7"/>
       <c r="AH37" s="7"/>
       <c r="AP37" s="6">
@@ -3097,8 +3112,14 @@
         <f>+Z38*1.05</f>
         <v>44708.332387354574</v>
       </c>
-      <c r="AE38" s="5"/>
-      <c r="AF38" s="5"/>
+      <c r="AE38" s="5">
+        <f>+AA38*1.05</f>
+        <v>44680.851063829788</v>
+      </c>
+      <c r="AF38" s="5">
+        <f>+AB38*1.05</f>
+        <v>43825.288992602873</v>
+      </c>
       <c r="AG38" s="5"/>
       <c r="AH38" s="5"/>
       <c r="AP38" s="5">
@@ -3286,8 +3307,12 @@
         <f>+Z40</f>
         <v>18212</v>
       </c>
-      <c r="AE40" s="5"/>
-      <c r="AF40" s="5"/>
+      <c r="AE40" s="5">
+        <v>17161</v>
+      </c>
+      <c r="AF40" s="5">
+        <v>13409</v>
+      </c>
       <c r="AG40" s="5"/>
       <c r="AH40" s="5"/>
       <c r="AP40" s="4">
@@ -3397,8 +3422,12 @@
         <f>+Y41</f>
         <v>416800</v>
       </c>
-      <c r="AE41" s="5"/>
-      <c r="AF41" s="5"/>
+      <c r="AE41" s="5">
+        <v>345454</v>
+      </c>
+      <c r="AF41" s="5">
+        <v>396835</v>
+      </c>
       <c r="AG41" s="5"/>
       <c r="AH41" s="5"/>
       <c r="AP41" s="4">
@@ -3530,8 +3559,14 @@
         <f>+Z42</f>
         <v>494989</v>
       </c>
-      <c r="AE42" s="7"/>
-      <c r="AF42" s="7"/>
+      <c r="AE42" s="7">
+        <f>+AE40+AE41</f>
+        <v>362615</v>
+      </c>
+      <c r="AF42" s="7">
+        <f>+AF40+AF41</f>
+        <v>410244</v>
+      </c>
       <c r="AG42" s="7"/>
       <c r="AH42" s="7"/>
       <c r="AP42" s="6">
@@ -3636,10 +3671,10 @@
       <c r="AF43" s="5"/>
       <c r="AG43" s="5"/>
       <c r="AH43" s="5"/>
-      <c r="AT43" s="26"/>
+      <c r="AT43" s="25"/>
     </row>
     <row r="44" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="40" t="s">
+      <c r="B44" s="39" t="s">
         <v>165</v>
       </c>
       <c r="C44" s="5"/>
@@ -3674,7 +3709,7 @@
       <c r="AF44" s="5"/>
       <c r="AG44" s="5"/>
       <c r="AH44" s="5"/>
-      <c r="AT44" s="26"/>
+      <c r="AT44" s="25"/>
       <c r="AU44" s="4">
         <f>+AU118-AT118</f>
         <v>573.50403199999982</v>
@@ -3775,7 +3810,7 @@
       <c r="S45" s="5">
         <v>15514</v>
       </c>
-      <c r="T45" s="12">
+      <c r="T45" s="11">
         <v>13670</v>
       </c>
       <c r="U45" s="5">
@@ -3800,7 +3835,7 @@
       <c r="AA45" s="5">
         <v>16460</v>
       </c>
-      <c r="AB45" s="36">
+      <c r="AB45" s="35">
         <v>18530</v>
       </c>
       <c r="AC45" s="5">
@@ -3814,7 +3849,9 @@
       <c r="AE45" s="5">
         <v>12925</v>
       </c>
-      <c r="AF45" s="5"/>
+      <c r="AF45" s="5">
+        <v>15787</v>
+      </c>
       <c r="AG45" s="5"/>
       <c r="AH45" s="5"/>
       <c r="AP45" s="4">
@@ -3829,7 +3866,7 @@
         <f>SUM(O45:R45)</f>
         <v>44125</v>
       </c>
-      <c r="AS45" s="39">
+      <c r="AS45" s="38">
         <f>SUM(S45:V45)</f>
         <v>68004</v>
       </c>
@@ -3972,7 +4009,9 @@
       <c r="AE46" s="5">
         <v>595</v>
       </c>
-      <c r="AF46" s="5"/>
+      <c r="AF46" s="5">
+        <v>439</v>
+      </c>
       <c r="AG46" s="5"/>
       <c r="AH46" s="5"/>
       <c r="AP46" s="4">
@@ -4086,7 +4125,9 @@
       <c r="AE47" s="5">
         <v>447</v>
       </c>
-      <c r="AF47" s="5"/>
+      <c r="AF47" s="5">
+        <v>435</v>
+      </c>
       <c r="AG47" s="5"/>
       <c r="AH47" s="5"/>
       <c r="AP47" s="4">
@@ -4183,7 +4224,7 @@
         <v>18692</v>
       </c>
       <c r="V48" s="7">
-        <f t="shared" ref="V48:AE48" si="41">SUM(V45:V47)</f>
+        <f t="shared" ref="V48:AF48" si="41">SUM(V45:V47)</f>
         <v>22353.8</v>
       </c>
       <c r="W48" s="7">
@@ -4222,7 +4263,10 @@
         <f t="shared" si="41"/>
         <v>13967</v>
       </c>
-      <c r="AF48" s="7"/>
+      <c r="AF48" s="7">
+        <f t="shared" si="41"/>
+        <v>16661</v>
+      </c>
       <c r="AG48" s="7"/>
       <c r="AH48" s="7"/>
       <c r="AP48" s="6">
@@ -4380,7 +4424,9 @@
       <c r="AE49" s="5">
         <v>2730</v>
       </c>
-      <c r="AF49" s="5"/>
+      <c r="AF49" s="5">
+        <v>2789</v>
+      </c>
       <c r="AG49" s="5"/>
       <c r="AH49" s="5"/>
       <c r="AJ49" s="4">
@@ -4503,7 +4549,9 @@
       <c r="AE50" s="5">
         <v>2638</v>
       </c>
-      <c r="AF50" s="5"/>
+      <c r="AF50" s="5">
+        <v>3046</v>
+      </c>
       <c r="AG50" s="5"/>
       <c r="AH50" s="5"/>
       <c r="AJ50" s="4">
@@ -4609,7 +4657,7 @@
         <v>21454</v>
       </c>
       <c r="V51" s="7">
-        <f t="shared" ref="V51:AE51" si="48">SUM(V48:V50)</f>
+        <f t="shared" ref="V51:AF51" si="48">SUM(V48:V50)</f>
         <v>24806.6</v>
       </c>
       <c r="W51" s="7">
@@ -4648,7 +4696,10 @@
         <f t="shared" si="48"/>
         <v>19335</v>
       </c>
-      <c r="AF51" s="7"/>
+      <c r="AF51" s="7">
+        <f t="shared" si="48"/>
+        <v>22496</v>
+      </c>
       <c r="AG51" s="7"/>
       <c r="AH51" s="7"/>
       <c r="AJ51" s="6">
@@ -4826,7 +4877,9 @@
       <c r="AE52" s="5">
         <v>11461</v>
       </c>
-      <c r="AF52" s="5"/>
+      <c r="AF52" s="5">
+        <v>13567</v>
+      </c>
       <c r="AG52" s="5"/>
       <c r="AH52" s="5"/>
       <c r="AJ52" s="4">
@@ -5001,7 +5054,10 @@
         <f>AE45-AE52</f>
         <v>1464</v>
       </c>
-      <c r="AF53" s="5"/>
+      <c r="AF53" s="5">
+        <f>AF45-AF52</f>
+        <v>2220</v>
+      </c>
       <c r="AG53" s="5"/>
       <c r="AH53" s="5"/>
       <c r="AR53" s="4">
@@ -5022,7 +5078,7 @@
       </c>
     </row>
     <row r="54" spans="2:58" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="29" t="s">
+      <c r="B54" s="28" t="s">
         <v>115</v>
       </c>
       <c r="C54" s="5"/>
@@ -5104,7 +5160,9 @@
       <c r="AE54" s="5">
         <v>0</v>
       </c>
-      <c r="AF54" s="5"/>
+      <c r="AF54" s="5">
+        <v>0</v>
+      </c>
       <c r="AG54" s="5"/>
       <c r="AH54" s="5"/>
       <c r="AU54" s="4">
@@ -5197,7 +5255,9 @@
       <c r="AE55" s="5">
         <v>239</v>
       </c>
-      <c r="AF55" s="5"/>
+      <c r="AF55" s="5">
+        <v>228</v>
+      </c>
       <c r="AG55" s="5"/>
       <c r="AH55" s="5"/>
       <c r="AS55" s="4">
@@ -5282,7 +5342,7 @@
         <v>5212</v>
       </c>
       <c r="V56" s="5">
-        <f t="shared" ref="V56:AE56" si="66">V48-V55-V52</f>
+        <f t="shared" ref="V56:AF56" si="66">V48-V55-V52</f>
         <v>6568.7999999999993</v>
       </c>
       <c r="W56" s="5">
@@ -5321,7 +5381,10 @@
         <f t="shared" si="66"/>
         <v>2267</v>
       </c>
-      <c r="AF56" s="5"/>
+      <c r="AF56" s="5">
+        <f t="shared" si="66"/>
+        <v>2866</v>
+      </c>
       <c r="AG56" s="5"/>
       <c r="AH56" s="5"/>
       <c r="AS56" s="4">
@@ -5466,7 +5529,9 @@
       <c r="AE57" s="5">
         <v>1945</v>
       </c>
-      <c r="AF57" s="5"/>
+      <c r="AF57" s="5">
+        <v>1943</v>
+      </c>
       <c r="AG57" s="5"/>
       <c r="AH57" s="5"/>
       <c r="AS57" s="4">
@@ -5567,7 +5632,9 @@
       <c r="AE58" s="5">
         <v>2537</v>
       </c>
-      <c r="AF58" s="5"/>
+      <c r="AF58" s="5">
+        <v>2880</v>
+      </c>
       <c r="AG58" s="5"/>
       <c r="AH58" s="5"/>
       <c r="AS58" s="4">
@@ -5648,7 +5715,7 @@
         <v>4233</v>
       </c>
       <c r="U59" s="5">
-        <f t="shared" ref="U59:AE59" si="71">U56+U49+U50-U57-U58</f>
+        <f t="shared" ref="U59:AF59" si="71">U56+U49+U50-U57-U58</f>
         <v>5382</v>
       </c>
       <c r="V59" s="5">
@@ -5691,7 +5758,10 @@
         <f t="shared" si="71"/>
         <v>3153</v>
       </c>
-      <c r="AF59" s="5"/>
+      <c r="AF59" s="5">
+        <f t="shared" si="71"/>
+        <v>3878</v>
+      </c>
       <c r="AG59" s="5"/>
       <c r="AH59" s="5"/>
       <c r="AS59" s="5">
@@ -5836,7 +5906,9 @@
       <c r="AE60" s="5">
         <v>1409</v>
       </c>
-      <c r="AF60" s="5"/>
+      <c r="AF60" s="5">
+        <v>1589</v>
+      </c>
       <c r="AG60" s="5"/>
       <c r="AH60" s="5"/>
       <c r="AS60" s="4">
@@ -5983,7 +6055,9 @@
         <f>1251+94</f>
         <v>1345</v>
       </c>
-      <c r="AF61" s="5"/>
+      <c r="AF61" s="5">
+        <v>1366</v>
+      </c>
       <c r="AG61" s="5"/>
       <c r="AH61" s="5"/>
       <c r="AS61" s="4">
@@ -6112,7 +6186,7 @@
         <v>1694</v>
       </c>
       <c r="V62" s="5">
-        <f t="shared" ref="V62:AE62" si="85">V60+V61</f>
+        <f t="shared" ref="V62:AF62" si="85">V60+V61</f>
         <v>2602.8000000000002</v>
       </c>
       <c r="W62" s="5">
@@ -6151,7 +6225,10 @@
         <f t="shared" si="85"/>
         <v>2754</v>
       </c>
-      <c r="AF62" s="5"/>
+      <c r="AF62" s="5">
+        <f t="shared" si="85"/>
+        <v>2955</v>
+      </c>
       <c r="AG62" s="5"/>
       <c r="AH62" s="5"/>
       <c r="AS62" s="4">
@@ -6319,7 +6396,10 @@
         <f>AE59-AE62</f>
         <v>399</v>
       </c>
-      <c r="AF63" s="5"/>
+      <c r="AF63" s="5">
+        <f>AF59-AF62</f>
+        <v>923</v>
+      </c>
       <c r="AG63" s="5"/>
       <c r="AH63" s="5"/>
       <c r="AS63" s="5">
@@ -6380,7 +6460,7 @@
       </c>
     </row>
     <row r="64" spans="2:58" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="40" t="s">
+      <c r="B64" s="39" t="s">
         <v>166</v>
       </c>
       <c r="C64" s="5"/>
@@ -6481,7 +6561,10 @@
         <f>400-91-119</f>
         <v>190</v>
       </c>
-      <c r="AF64" s="5"/>
+      <c r="AF64" s="5">
+        <f>392-86+320</f>
+        <v>626</v>
+      </c>
       <c r="AG64" s="5"/>
       <c r="AH64" s="5"/>
       <c r="AT64" s="4">
@@ -6606,7 +6689,7 @@
         <v>3636</v>
       </c>
       <c r="V65" s="5">
-        <f t="shared" ref="V65:AE65" si="103">V63+V64</f>
+        <f t="shared" ref="V65:AF65" si="103">V63+V64</f>
         <v>3744.7999999999984</v>
       </c>
       <c r="W65" s="5">
@@ -6645,7 +6728,10 @@
         <f t="shared" si="103"/>
         <v>589</v>
       </c>
-      <c r="AF65" s="5"/>
+      <c r="AF65" s="5">
+        <f t="shared" si="103"/>
+        <v>1549</v>
+      </c>
       <c r="AG65" s="5"/>
       <c r="AH65" s="5"/>
       <c r="AT65" s="4">
@@ -6806,7 +6892,10 @@
         <f>169+11</f>
         <v>180</v>
       </c>
-      <c r="AF66" s="5"/>
+      <c r="AF66" s="35">
+        <f>359+18</f>
+        <v>377</v>
+      </c>
       <c r="AG66" s="5"/>
       <c r="AH66" s="5"/>
       <c r="AT66" s="4">
@@ -6931,7 +7020,7 @@
         <v>3331</v>
       </c>
       <c r="V67" s="5">
-        <f t="shared" ref="V67:AE67" si="110">V65-V66</f>
+        <f t="shared" ref="V67:AF67" si="110">V65-V66</f>
         <v>3468.7999999999984</v>
       </c>
       <c r="W67" s="5">
@@ -6970,7 +7059,10 @@
         <f t="shared" si="110"/>
         <v>409</v>
       </c>
-      <c r="AF67" s="5"/>
+      <c r="AF67" s="5">
+        <f t="shared" si="110"/>
+        <v>1172</v>
+      </c>
       <c r="AG67" s="5"/>
       <c r="AH67" s="5"/>
       <c r="AT67" s="4">
@@ -7299,7 +7391,7 @@
         <v>0.96049596309111884</v>
       </c>
       <c r="V68" s="3">
-        <f t="shared" ref="V68:AE68" si="123">V67/V69</f>
+        <f t="shared" ref="V68:AF68" si="123">V67/V69</f>
         <v>0.99936617689426632</v>
       </c>
       <c r="W68" s="3">
@@ -7338,58 +7430,61 @@
         <f t="shared" si="123"/>
         <v>0.12709757613424488</v>
       </c>
-      <c r="AF68" s="3"/>
+      <c r="AF68" s="3">
+        <f t="shared" si="123"/>
+        <v>0.36363636363636365</v>
+      </c>
       <c r="AG68" s="3"/>
       <c r="AH68" s="3"/>
-      <c r="AT68" s="20">
+      <c r="AT68" s="19">
         <f>+AT67/AT69</f>
         <v>2.6545115210681214</v>
       </c>
-      <c r="AU68" s="20">
+      <c r="AU68" s="19">
         <f t="shared" ref="AU68:BA68" si="124">+AU67/AU69</f>
         <v>1.6780011264731298</v>
       </c>
-      <c r="AV68" s="20">
+      <c r="AV68" s="19">
         <f t="shared" si="124"/>
         <v>3.7395404610724348</v>
       </c>
-      <c r="AW68" s="20">
+      <c r="AW68" s="19">
         <f t="shared" si="124"/>
         <v>6.4209756583989677</v>
       </c>
-      <c r="AX68" s="20">
+      <c r="AX68" s="19">
         <f t="shared" si="124"/>
         <v>8.7301028185899359</v>
       </c>
-      <c r="AY68" s="20">
+      <c r="AY68" s="19">
         <f t="shared" si="124"/>
         <v>12.590795261194229</v>
       </c>
-      <c r="AZ68" s="20">
+      <c r="AZ68" s="19">
         <f t="shared" si="124"/>
         <v>16.972403893738136</v>
       </c>
-      <c r="BA68" s="20">
+      <c r="BA68" s="19">
         <f t="shared" si="124"/>
         <v>21.586249774527918</v>
       </c>
-      <c r="BB68" s="20">
+      <c r="BB68" s="19">
         <f t="shared" ref="BB68:BF68" si="125">+BB67/BB69</f>
         <v>24.935077210470315</v>
       </c>
-      <c r="BC68" s="20">
+      <c r="BC68" s="19">
         <f t="shared" si="125"/>
         <v>28.69252784225354</v>
       </c>
-      <c r="BD68" s="20">
+      <c r="BD68" s="19">
         <f t="shared" si="125"/>
         <v>32.90321060848143</v>
       </c>
-      <c r="BE68" s="20">
+      <c r="BE68" s="19">
         <f t="shared" si="125"/>
         <v>37.616307381369978</v>
       </c>
-      <c r="BF68" s="20">
+      <c r="BF68" s="19">
         <f t="shared" si="125"/>
         <v>42.886023550381566</v>
       </c>
@@ -7484,7 +7579,9 @@
       <c r="AE69" s="5">
         <v>3218</v>
       </c>
-      <c r="AF69" s="5"/>
+      <c r="AF69" s="5">
+        <v>3223</v>
+      </c>
       <c r="AG69" s="5"/>
       <c r="AH69" s="5"/>
       <c r="AT69" s="4">
@@ -7540,934 +7637,952 @@
         <v>3481.75</v>
       </c>
     </row>
-    <row r="71" spans="2:109" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="23" t="s">
+    <row r="71" spans="2:109" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="C71" s="24"/>
-      <c r="D71" s="24"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="24"/>
-      <c r="G71" s="24"/>
-      <c r="H71" s="24"/>
-      <c r="I71" s="24"/>
-      <c r="J71" s="24"/>
-      <c r="K71" s="22">
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="23"/>
+      <c r="G71" s="23"/>
+      <c r="H71" s="23"/>
+      <c r="I71" s="23"/>
+      <c r="J71" s="23"/>
+      <c r="K71" s="21">
         <f>K51/G51-1</f>
         <v>0.31799163179916312</v>
       </c>
-      <c r="L71" s="22">
+      <c r="L71" s="21">
         <f t="shared" ref="L71" si="133">L51/H51-1</f>
         <v>-4.9448818897637747E-2</v>
       </c>
-      <c r="M71" s="22">
+      <c r="M71" s="21">
         <f t="shared" ref="M71" si="134">M51/I51-1</f>
         <v>0.39155957480564818</v>
       </c>
-      <c r="N71" s="22">
+      <c r="N71" s="21">
         <f t="shared" ref="N71" si="135">N51/J51-1</f>
         <v>0.45503791982665232</v>
       </c>
-      <c r="O71" s="22">
+      <c r="O71" s="21">
         <f t="shared" ref="O71" si="136">O51/K51-1</f>
         <v>0.73583959899749374</v>
       </c>
-      <c r="P71" s="22">
+      <c r="P71" s="21">
         <f t="shared" ref="P71:Q71" si="137">P51/L51-1</f>
         <v>0.98111332007952279</v>
       </c>
-      <c r="Q71" s="22">
+      <c r="Q71" s="21">
         <f t="shared" si="137"/>
         <v>0.56846425721126437</v>
       </c>
-      <c r="R71" s="22">
+      <c r="R71" s="21">
         <f t="shared" ref="R71:S71" si="138">R51/N51-1</f>
         <v>0.64919955323901712</v>
       </c>
-      <c r="S71" s="22">
+      <c r="S71" s="21">
         <f t="shared" si="138"/>
         <v>0.80537106555010096</v>
       </c>
-      <c r="T71" s="22">
+      <c r="T71" s="21">
         <f>T51/P51-1</f>
         <v>0.41612309750794441</v>
       </c>
-      <c r="U71" s="22">
+      <c r="U71" s="21">
         <f>U51/Q51-1</f>
         <v>0.55949698335392894</v>
       </c>
-      <c r="V71" s="22">
+      <c r="V71" s="21">
         <f>V51/R51-1</f>
         <v>0.39999999999999991</v>
       </c>
-      <c r="W71" s="22">
-        <f t="shared" ref="W71:AE71" si="139">W51/S51-1</f>
+      <c r="W71" s="21">
+        <f t="shared" ref="W71:AF71" si="139">W51/S51-1</f>
         <v>0.24381531243335464</v>
       </c>
-      <c r="X71" s="22">
+      <c r="X71" s="21">
         <f t="shared" si="139"/>
         <v>0.47200897602456604</v>
       </c>
-      <c r="Y71" s="22">
+      <c r="Y71" s="21">
         <f t="shared" si="139"/>
         <v>8.8375128181224838E-2</v>
       </c>
-      <c r="Z71" s="22">
+      <c r="Z71" s="21">
         <f>Z51/V51-1</f>
         <v>1.452839163770947E-2</v>
       </c>
-      <c r="AA71" s="22">
+      <c r="AA71" s="21">
         <f>AA51/W51-1</f>
         <v>-8.6930429936988296E-2</v>
       </c>
-      <c r="AB71" s="22">
+      <c r="AB71" s="21">
         <f t="shared" si="139"/>
         <v>2.2987122397400306E-2</v>
       </c>
-      <c r="AC71" s="22">
+      <c r="AC71" s="21">
         <f t="shared" si="139"/>
         <v>0.11765334961430951</v>
       </c>
-      <c r="AD71" s="22">
+      <c r="AD71" s="21">
         <f t="shared" si="139"/>
         <v>0.13521798932415607</v>
       </c>
-      <c r="AE71" s="22">
+      <c r="AE71" s="21">
         <f t="shared" si="139"/>
         <v>-9.2296136331627587E-2</v>
       </c>
-      <c r="AF71" s="22"/>
-      <c r="AG71" s="22"/>
-      <c r="AH71" s="22"/>
-      <c r="AK71" s="25">
+      <c r="AF71" s="21">
+        <f t="shared" si="139"/>
+        <v>-0.1178039215686274</v>
+      </c>
+      <c r="AG71" s="21"/>
+      <c r="AH71" s="21"/>
+      <c r="AK71" s="24">
         <f t="shared" ref="AK71:AM71" si="140">AK51/AJ51-1</f>
         <v>0.58845907814070664</v>
       </c>
-      <c r="AL71" s="25">
+      <c r="AL71" s="24">
         <f t="shared" si="140"/>
         <v>0.26503272306147285</v>
       </c>
-      <c r="AM71" s="25">
+      <c r="AM71" s="24">
         <f t="shared" si="140"/>
         <v>0.73012574069611524</v>
       </c>
-      <c r="AN71" s="25">
+      <c r="AN71" s="24">
         <f>AN51/AM51-1</f>
         <v>0.67978989539054413</v>
       </c>
-      <c r="AO71" s="25">
+      <c r="AO71" s="24">
         <f>AO51/AN51-1</f>
         <v>0.82513159773516764</v>
       </c>
-      <c r="AP71" s="25">
+      <c r="AP71" s="24">
         <f>AP51/AO51-1</f>
         <v>0.14522590184326489</v>
       </c>
-      <c r="AQ71" s="25">
+      <c r="AQ71" s="24">
         <f>+AQ51/AP51-1</f>
         <v>0.28309870615998056</v>
       </c>
-      <c r="AR71" s="25">
+      <c r="AR71" s="24">
         <f>+AR51/AQ51-1</f>
         <v>0.70671613394216126</v>
       </c>
-      <c r="AS71" s="25">
+      <c r="AS71" s="24">
         <f>+AS51/AR51-1</f>
         <v>0.52259442989056737</v>
       </c>
-      <c r="AT71" s="25">
+      <c r="AT71" s="24">
         <f>+AT51/AS51-1</f>
         <v>0.18086993871917945</v>
       </c>
-      <c r="AU71" s="25">
+      <c r="AU71" s="24">
         <f t="shared" ref="AU71:AY71" si="141">+AU51/AT51-1</f>
         <v>5.444432726912618E-2</v>
       </c>
-      <c r="AV71" s="25">
+      <c r="AV71" s="24">
         <f t="shared" si="141"/>
         <v>-2.3848604099481197E-2</v>
       </c>
-      <c r="AW71" s="25">
+      <c r="AW71" s="24">
         <f t="shared" si="141"/>
         <v>0.2988437649339839</v>
       </c>
-      <c r="AX71" s="25">
+      <c r="AX71" s="24">
         <f t="shared" si="141"/>
         <v>0.24522052781689352</v>
       </c>
-      <c r="AY71" s="25">
+      <c r="AY71" s="24">
         <f t="shared" si="141"/>
         <v>0.24429471024781169</v>
       </c>
-      <c r="AZ71" s="25">
+      <c r="AZ71" s="24">
         <f t="shared" ref="AZ71:BA71" si="142">+AZ51/AY51-1</f>
         <v>0.19142450022795243</v>
       </c>
-      <c r="BA71" s="25">
+      <c r="BA71" s="24">
         <f t="shared" si="142"/>
         <v>0.1388373668361893</v>
       </c>
-      <c r="BB71" s="25">
+      <c r="BB71" s="24">
         <f t="shared" ref="BB71" si="143">+BB51/BA51-1</f>
         <v>8.173446995315059E-2</v>
       </c>
-      <c r="BC71" s="25">
+      <c r="BC71" s="24">
         <f t="shared" ref="BC71" si="144">+BC51/BB51-1</f>
         <v>8.1665310206848085E-2</v>
       </c>
-      <c r="BD71" s="25">
+      <c r="BD71" s="24">
         <f t="shared" ref="BD71" si="145">+BD51/BC51-1</f>
         <v>8.1600781805080569E-2</v>
       </c>
-      <c r="BE71" s="25">
+      <c r="BE71" s="24">
         <f t="shared" ref="BE71" si="146">+BE51/BD51-1</f>
         <v>8.1540603100230369E-2</v>
       </c>
-      <c r="BF71" s="25">
+      <c r="BF71" s="24">
         <f t="shared" ref="BF71" si="147">+BF51/BE51-1</f>
         <v>8.1484511217818634E-2</v>
       </c>
     </row>
     <row r="72" spans="2:109" x14ac:dyDescent="0.2">
-      <c r="B72" s="21" t="s">
+      <c r="B72" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="K72" s="17">
-        <f t="shared" ref="K72:AE72" si="148">+K37/G37-1</f>
+      <c r="K72" s="16">
+        <f t="shared" ref="K72:AF72" si="148">+K37/G37-1</f>
         <v>0.40427490122026688</v>
       </c>
-      <c r="L72" s="17">
+      <c r="L72" s="16">
         <f t="shared" si="148"/>
         <v>-4.9351902344897058E-2</v>
       </c>
-      <c r="M72" s="17">
+      <c r="M72" s="16">
         <f t="shared" si="148"/>
         <v>0.43333401930319182</v>
       </c>
-      <c r="N72" s="17">
+      <c r="N72" s="16">
         <f t="shared" si="148"/>
         <v>0.61086578348722065</v>
       </c>
-      <c r="O72" s="17">
+      <c r="O72" s="16">
         <f t="shared" si="148"/>
         <v>1.088229976496113</v>
       </c>
-      <c r="P72" s="17">
+      <c r="P72" s="16">
         <f t="shared" si="148"/>
         <v>1.2200772200772199</v>
       </c>
-      <c r="Q72" s="17">
+      <c r="Q72" s="16">
         <f t="shared" si="148"/>
         <v>0.73223259152907394</v>
       </c>
-      <c r="R72" s="17">
+      <c r="R72" s="16">
         <f t="shared" si="148"/>
         <v>0.70903250816857732</v>
       </c>
-      <c r="S72" s="17">
+      <c r="S72" s="16">
         <f t="shared" si="148"/>
         <v>0.67774891774891777</v>
       </c>
-      <c r="T72" s="17">
+      <c r="T72" s="16">
         <f t="shared" si="148"/>
         <v>0.26556521739130434</v>
       </c>
-      <c r="U72" s="17">
+      <c r="U72" s="16">
         <f t="shared" si="148"/>
         <v>0.42490675507666809</v>
       </c>
-      <c r="V72" s="17">
+      <c r="V72" s="16">
         <f t="shared" si="148"/>
         <v>0.31327932598833441</v>
       </c>
-      <c r="W72" s="17">
+      <c r="W72" s="16">
         <f t="shared" si="148"/>
         <v>0.36390171844359576</v>
       </c>
-      <c r="X72" s="17">
+      <c r="X72" s="16">
         <f t="shared" si="148"/>
         <v>0.83018904964761764</v>
       </c>
-      <c r="Y72" s="17">
+      <c r="Y72" s="16">
         <f t="shared" si="148"/>
         <v>0.26533170462146982</v>
       </c>
-      <c r="Z72" s="17">
+      <c r="Z72" s="16">
         <f t="shared" si="148"/>
         <v>0.19549297025745282</v>
       </c>
-      <c r="AA72" s="17">
+      <c r="AA72" s="16">
         <f t="shared" si="148"/>
         <v>-8.5285249778303318E-2</v>
       </c>
-      <c r="AB72" s="17">
+      <c r="AB72" s="16">
         <f t="shared" si="148"/>
         <v>-4.7590852533573647E-2</v>
       </c>
-      <c r="AC72" s="17">
+      <c r="AC72" s="16">
         <f t="shared" si="148"/>
         <v>0.10358411158026848</v>
       </c>
-      <c r="AD72" s="17">
+      <c r="AD72" s="16">
         <f t="shared" si="148"/>
         <v>0.10948139036174909</v>
       </c>
-      <c r="AE72" s="17">
+      <c r="AE72" s="16">
         <f t="shared" si="148"/>
-        <v>-1</v>
-      </c>
-      <c r="AF72" s="17"/>
-      <c r="AG72" s="17"/>
-      <c r="AH72" s="17"/>
-      <c r="AQ72" s="26">
+        <v>-0.12959592564825106</v>
+      </c>
+      <c r="AF72" s="16">
+        <f t="shared" si="148"/>
+        <v>-0.13477461730441753</v>
+      </c>
+      <c r="AG72" s="16"/>
+      <c r="AH72" s="16"/>
+      <c r="AQ72" s="25">
         <f t="shared" ref="AQ72:BA72" si="149">+AQ37/AP37-1</f>
         <v>0.35729051069477991</v>
       </c>
-      <c r="AR72" s="26">
+      <c r="AR72" s="25">
         <f t="shared" si="149"/>
         <v>0.87559116340959009</v>
       </c>
-      <c r="AS72" s="26">
+      <c r="AS72" s="25">
         <f t="shared" si="149"/>
         <v>0.403761953095785</v>
       </c>
-      <c r="AT72" s="26">
+      <c r="AT72" s="25">
         <f t="shared" si="149"/>
         <v>0.37654954785588313</v>
       </c>
-      <c r="AU72" s="26">
+      <c r="AU72" s="25">
         <f t="shared" si="149"/>
         <v>2.2039764876441881E-2</v>
       </c>
-      <c r="AV72" s="26">
+      <c r="AV72" s="25">
         <f t="shared" si="149"/>
         <v>0.20593650208172676</v>
       </c>
-      <c r="AW72" s="26">
+      <c r="AW72" s="25">
         <f t="shared" si="149"/>
         <v>0.25</v>
       </c>
-      <c r="AX72" s="26">
+      <c r="AX72" s="25">
         <f t="shared" si="149"/>
         <v>0.19999999999999996</v>
       </c>
-      <c r="AY72" s="26">
+      <c r="AY72" s="25">
         <f t="shared" si="149"/>
         <v>0.19999999999999996</v>
       </c>
-      <c r="AZ72" s="26">
+      <c r="AZ72" s="25">
         <f t="shared" si="149"/>
         <v>0.14999999999999991</v>
       </c>
-      <c r="BA72" s="26">
+      <c r="BA72" s="25">
         <f t="shared" si="149"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="BB72" s="26">
+      <c r="BB72" s="25">
         <f t="shared" ref="BB72:BF72" si="150">+BB37/BA37-1</f>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="BC72" s="26">
+      <c r="BC72" s="25">
         <f t="shared" si="150"/>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="BD72" s="26">
+      <c r="BD72" s="25">
         <f t="shared" si="150"/>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="BE72" s="26">
+      <c r="BE72" s="25">
         <f t="shared" si="150"/>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="BF72" s="26">
+      <c r="BF72" s="25">
         <f t="shared" si="150"/>
         <v>5.0000000000000044E-2</v>
       </c>
     </row>
     <row r="73" spans="2:109" x14ac:dyDescent="0.2">
-      <c r="B73" s="21" t="s">
+      <c r="B73" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="K73" s="17">
-        <f t="shared" ref="K73:AE73" si="151">+K42/G42-1</f>
+      <c r="K73" s="16">
+        <f t="shared" ref="K73:AF73" si="151">+K42/G42-1</f>
         <v>0.33101713811610356</v>
       </c>
-      <c r="L73" s="17">
+      <c r="L73" s="16">
         <f t="shared" si="151"/>
         <v>-5.4866280672732248E-2</v>
       </c>
-      <c r="M73" s="17">
+      <c r="M73" s="16">
         <f t="shared" si="151"/>
         <v>0.50835629972440333</v>
       </c>
-      <c r="N73" s="17">
+      <c r="N73" s="16">
         <f t="shared" si="151"/>
         <v>0.71375046476818782</v>
       </c>
-      <c r="O73" s="17">
+      <c r="O73" s="16">
         <f t="shared" si="151"/>
         <v>0.75644771700171409</v>
       </c>
-      <c r="P73" s="17">
+      <c r="P73" s="16">
         <f t="shared" si="151"/>
         <v>1.5090067094515751</v>
       </c>
-      <c r="Q73" s="17">
+      <c r="Q73" s="16">
         <f t="shared" si="151"/>
         <v>0.63975150996993846</v>
       </c>
-      <c r="R73" s="17">
+      <c r="R73" s="16">
         <f t="shared" si="151"/>
         <v>0.7014080119272128</v>
       </c>
-      <c r="S73" s="17">
+      <c r="S73" s="16">
         <f t="shared" si="151"/>
         <v>0.69352549102241356</v>
       </c>
-      <c r="T73" s="17">
+      <c r="T73" s="16">
         <f t="shared" si="151"/>
         <v>0.25268262434539124</v>
       </c>
-      <c r="U73" s="17">
+      <c r="U73" s="16">
         <f t="shared" si="151"/>
         <v>0.53863587626091669</v>
       </c>
-      <c r="V73" s="17">
+      <c r="V73" s="16">
         <f t="shared" si="151"/>
         <v>0.43768310227569973</v>
       </c>
-      <c r="W73" s="17">
+      <c r="W73" s="16">
         <f t="shared" si="151"/>
         <v>0.44334609226376598</v>
       </c>
-      <c r="X73" s="17">
+      <c r="X73" s="16">
         <f t="shared" si="151"/>
         <v>0.85513187408152214</v>
       </c>
-      <c r="Y73" s="17">
+      <c r="Y73" s="16">
         <f t="shared" si="151"/>
         <v>0.17644422460462983</v>
       </c>
-      <c r="Z73" s="17">
+      <c r="Z73" s="16">
         <f t="shared" si="151"/>
         <v>0.12573999149421988</v>
       </c>
-      <c r="AA73" s="17">
+      <c r="AA73" s="16">
         <f t="shared" si="151"/>
         <v>-1.687129090216144E-2</v>
       </c>
-      <c r="AB73" s="17">
+      <c r="AB73" s="16">
         <f t="shared" si="151"/>
         <v>-0.14356681259120285</v>
       </c>
-      <c r="AC73" s="17">
+      <c r="AC73" s="16">
         <f t="shared" si="151"/>
         <v>1.159813978554558E-2</v>
       </c>
-      <c r="AD73" s="17">
+      <c r="AD73" s="16">
         <f t="shared" si="151"/>
         <v>0</v>
       </c>
-      <c r="AE73" s="17">
+      <c r="AE73" s="16">
         <f t="shared" si="151"/>
-        <v>-1</v>
-      </c>
-      <c r="AF73" s="17"/>
-      <c r="AG73" s="17"/>
-      <c r="AH73" s="17"/>
-      <c r="AQ73" s="26">
+        <v>-0.16326888508921922</v>
+      </c>
+      <c r="AF73" s="16">
+        <f t="shared" si="151"/>
+        <v>-1.4288113603890817E-3</v>
+      </c>
+      <c r="AG73" s="16"/>
+      <c r="AH73" s="16"/>
+      <c r="AQ73" s="25">
         <f t="shared" ref="AQ73:BA73" si="152">+AQ42/AP42-1</f>
         <v>0.39565262627590125</v>
       </c>
-      <c r="AR73" s="26">
+      <c r="AR73" s="25">
         <f t="shared" si="152"/>
         <v>0.8252981439448186</v>
       </c>
-      <c r="AS73" s="26">
+      <c r="AS73" s="25">
         <f t="shared" si="152"/>
         <v>0.47203204567389845</v>
       </c>
-      <c r="AT73" s="26">
+      <c r="AT73" s="25">
         <f t="shared" si="152"/>
         <v>0.34781700789494252</v>
       </c>
-      <c r="AU73" s="26">
+      <c r="AU73" s="25">
         <f t="shared" si="152"/>
         <v>-7.1121997199327103E-2</v>
       </c>
-      <c r="AV73" s="26">
+      <c r="AV73" s="25">
         <f t="shared" si="152"/>
         <v>0.30000000000000027</v>
       </c>
-      <c r="AW73" s="26">
+      <c r="AW73" s="25">
         <f t="shared" si="152"/>
         <v>0.25</v>
       </c>
-      <c r="AX73" s="26">
+      <c r="AX73" s="25">
         <f t="shared" si="152"/>
         <v>0.19999999999999996</v>
       </c>
-      <c r="AY73" s="26">
+      <c r="AY73" s="25">
         <f t="shared" si="152"/>
         <v>0.19999999999999996</v>
       </c>
-      <c r="AZ73" s="26">
+      <c r="AZ73" s="25">
         <f t="shared" si="152"/>
         <v>0.14999999999999991</v>
       </c>
-      <c r="BA73" s="26">
+      <c r="BA73" s="25">
         <f t="shared" si="152"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="BB73" s="26">
+      <c r="BB73" s="25">
         <f t="shared" ref="BB73:BF73" si="153">+BB42/BA42-1</f>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="BC73" s="26">
+      <c r="BC73" s="25">
         <f t="shared" si="153"/>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="BD73" s="26">
+      <c r="BD73" s="25">
         <f t="shared" si="153"/>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="BE73" s="26">
+      <c r="BE73" s="25">
         <f t="shared" si="153"/>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="BF73" s="26">
+      <c r="BF73" s="25">
         <f t="shared" si="153"/>
         <v>5.0000000000000044E-2</v>
       </c>
     </row>
     <row r="74" spans="2:109" x14ac:dyDescent="0.2">
-      <c r="B74" s="19" t="s">
+      <c r="B74" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="K74" s="17">
+      <c r="K74" s="16">
         <f t="shared" ref="K74:O74" si="154">K45/G45-1</f>
         <v>0.39441436306640076</v>
       </c>
-      <c r="L74" s="17">
+      <c r="L74" s="16">
         <f t="shared" si="154"/>
         <v>-4.9729102167182626E-2</v>
       </c>
-      <c r="M74" s="17">
+      <c r="M74" s="16">
         <f t="shared" si="154"/>
         <v>0.43141075604053003</v>
       </c>
-      <c r="N74" s="17">
+      <c r="N74" s="16">
         <f t="shared" si="154"/>
         <v>0.4053394107113788</v>
       </c>
-      <c r="O74" s="17">
+      <c r="O74" s="16">
         <f t="shared" si="154"/>
         <v>0.67320662170447587</v>
       </c>
-      <c r="P74" s="17">
+      <c r="P74" s="16">
         <f>P45/L45-1</f>
         <v>0.9385053960496843</v>
       </c>
-      <c r="Q74" s="17">
+      <c r="Q74" s="16">
         <f t="shared" ref="Q74" si="155">Q45/M45-1</f>
         <v>0.55091206098557044</v>
       </c>
-      <c r="R74" s="17">
+      <c r="R74" s="16">
         <f>R45/N45-1</f>
         <v>0.74041468782578468</v>
       </c>
-      <c r="S74" s="17">
+      <c r="S74" s="16">
         <f t="shared" ref="S74:U74" si="156">S45/O45-1</f>
         <v>0.89495541712470983</v>
       </c>
-      <c r="T74" s="17">
+      <c r="T74" s="16">
         <f t="shared" si="156"/>
         <v>0.43592436974789917</v>
       </c>
-      <c r="U74" s="17">
+      <c r="U74" s="16">
         <f t="shared" si="156"/>
         <v>0.561046256473273</v>
       </c>
-      <c r="V74" s="17">
+      <c r="V74" s="16">
         <f t="shared" ref="V74" si="157">V45/R45-1</f>
         <v>0.39999999999999991</v>
       </c>
-      <c r="W74" s="17">
+      <c r="W74" s="16">
         <f>W45/S45-1</f>
         <v>0.21683640582699493</v>
       </c>
-      <c r="X74" s="17">
+      <c r="X74" s="16">
         <f t="shared" ref="X74" si="158">X45/T45-1</f>
         <v>0.49370885149963417</v>
       </c>
-      <c r="Y74" s="17">
+      <c r="Y74" s="16">
         <f t="shared" ref="Y74" si="159">Y45/U45-1</f>
         <v>4.4813044700590332E-2</v>
       </c>
-      <c r="Z74" s="17">
-        <f t="shared" ref="Z74:AE74" si="160">Z45/V45-1</f>
+      <c r="Z74" s="16">
+        <f t="shared" ref="Z74:AF74" si="160">Z45/V45-1</f>
         <v>-1.9253624910862799E-2</v>
       </c>
-      <c r="AA74" s="17">
+      <c r="AA74" s="16">
         <f t="shared" si="160"/>
         <v>-0.12808560228837795</v>
       </c>
-      <c r="AB74" s="17">
+      <c r="AB74" s="16">
         <f>AB45/X45-1</f>
         <v>-9.2511876193741127E-2</v>
       </c>
-      <c r="AC74" s="17">
+      <c r="AC74" s="16">
         <f t="shared" si="160"/>
         <v>6.7657179716614557E-2</v>
       </c>
-      <c r="AD74" s="17">
+      <c r="AD74" s="16">
         <f t="shared" si="160"/>
         <v>0.16495545987983684</v>
       </c>
-      <c r="AE74" s="17">
+      <c r="AE74" s="16">
         <f t="shared" si="160"/>
         <v>-0.21476306196840822</v>
       </c>
-      <c r="AF74" s="17"/>
-      <c r="AG74" s="17"/>
-      <c r="AH74" s="17"/>
+      <c r="AF74" s="16">
+        <f t="shared" si="160"/>
+        <v>-0.14803022126281706</v>
+      </c>
+      <c r="AG74" s="16"/>
+      <c r="AH74" s="16"/>
     </row>
     <row r="75" spans="2:109" x14ac:dyDescent="0.2">
-      <c r="B75" s="19" t="s">
+      <c r="B75" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C75" s="17"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="17"/>
-      <c r="F75" s="17"/>
-      <c r="G75" s="17">
+      <c r="C75" s="16"/>
+      <c r="D75" s="16"/>
+      <c r="E75" s="16"/>
+      <c r="F75" s="16"/>
+      <c r="G75" s="16">
         <f t="shared" ref="G75:K75" si="161">G53/G45</f>
         <v>0.18609290396124251</v>
       </c>
-      <c r="H75" s="17">
+      <c r="H75" s="16">
         <f t="shared" si="161"/>
         <v>0.17685758513931887</v>
       </c>
-      <c r="I75" s="17">
+      <c r="I75" s="16">
         <f t="shared" si="161"/>
         <v>0.21784879189399844</v>
       </c>
-      <c r="J75" s="17">
+      <c r="J75" s="16">
         <f t="shared" si="161"/>
         <v>0.21618101904606871</v>
       </c>
-      <c r="K75" s="17">
+      <c r="K75" s="16">
         <f t="shared" si="161"/>
         <v>0.2440220723482526</v>
       </c>
-      <c r="L75" s="17">
+      <c r="L75" s="16">
         <f t="shared" ref="L75" si="162">L53/L45</f>
         <v>0.24373854612095297</v>
       </c>
-      <c r="M75" s="17">
+      <c r="M75" s="16">
         <f t="shared" ref="M75" si="163">M53/M45</f>
         <v>0.27021508303838826</v>
       </c>
-      <c r="N75" s="17">
+      <c r="N75" s="16">
         <f t="shared" ref="N75:U75" si="164">N53/N45</f>
         <v>0.19819298042395458</v>
       </c>
-      <c r="O75" s="17">
+      <c r="O75" s="16">
         <f t="shared" si="164"/>
         <v>0.21131061438866497</v>
       </c>
-      <c r="P75" s="17">
+      <c r="P75" s="16">
         <f t="shared" si="164"/>
         <v>0.25220588235294117</v>
       </c>
-      <c r="Q75" s="17">
+      <c r="Q75" s="16">
         <f t="shared" si="164"/>
         <v>0.28464846835776353</v>
       </c>
-      <c r="R75" s="17">
+      <c r="R75" s="16">
         <f t="shared" si="164"/>
         <v>0.28858569051580701</v>
       </c>
-      <c r="S75" s="17">
+      <c r="S75" s="16">
         <f t="shared" si="164"/>
         <v>0.29650638133298957</v>
       </c>
-      <c r="T75" s="17">
+      <c r="T75" s="16">
         <f t="shared" si="164"/>
         <v>0.25727871250914414</v>
       </c>
-      <c r="U75" s="17">
+      <c r="U75" s="16">
         <f t="shared" si="164"/>
         <v>0.26348046106269329</v>
       </c>
-      <c r="V75" s="17">
+      <c r="V75" s="16">
         <f t="shared" ref="V75:AD75" si="165">V53/V45</f>
         <v>0.26631804135963871</v>
       </c>
-      <c r="W75" s="17">
+      <c r="W75" s="16">
         <f>W53/W45</f>
         <v>0.1830702404915775</v>
       </c>
-      <c r="X75" s="17">
+      <c r="X75" s="16">
         <f t="shared" si="165"/>
         <v>0.17522895342573094</v>
       </c>
-      <c r="Y75" s="17">
+      <c r="Y75" s="16">
         <f t="shared" si="165"/>
         <v>0.15746421267893659</v>
       </c>
-      <c r="Z75" s="17">
+      <c r="Z75" s="16">
         <f t="shared" si="165"/>
         <v>0.16616577799321378</v>
       </c>
-      <c r="AA75" s="17">
+      <c r="AA75" s="16">
         <f t="shared" si="165"/>
         <v>0.15571081409477522</v>
       </c>
-      <c r="AB75" s="17">
+      <c r="AB75" s="16">
         <f t="shared" si="165"/>
         <v>0.13858607663248787</v>
       </c>
-      <c r="AC75" s="17">
+      <c r="AC75" s="16">
         <f t="shared" si="165"/>
         <v>0.15000000000000002</v>
       </c>
-      <c r="AD75" s="17">
+      <c r="AD75" s="16">
         <f t="shared" si="165"/>
         <v>0.15000000000000002</v>
       </c>
-      <c r="AE75" s="17">
-        <f t="shared" ref="AE75" si="166">AE53/AE45</f>
+      <c r="AE75" s="16">
+        <f t="shared" ref="AE75:AF75" si="166">AE53/AE45</f>
         <v>0.1132688588007737</v>
       </c>
-      <c r="AF75" s="17"/>
-      <c r="AG75" s="17"/>
-      <c r="AH75" s="17"/>
-      <c r="AQ75" s="17">
+      <c r="AF75" s="16">
+        <f t="shared" si="166"/>
+        <v>0.14062203078482297</v>
+      </c>
+      <c r="AG75" s="16"/>
+      <c r="AH75" s="16"/>
+      <c r="AQ75" s="16">
         <f t="shared" ref="AQ75:AU75" si="167">AQ53/AQ45</f>
         <v>0</v>
       </c>
-      <c r="AR75" s="17">
+      <c r="AR75" s="16">
         <f t="shared" si="167"/>
         <v>0.38841926345609062</v>
       </c>
-      <c r="AS75" s="17">
+      <c r="AS75" s="16">
         <f t="shared" si="167"/>
         <v>0.27064584436209632</v>
       </c>
-      <c r="AT75" s="17">
+      <c r="AT75" s="16">
         <f t="shared" si="167"/>
         <v>0.17052821969455731</v>
       </c>
-      <c r="AU75" s="17">
+      <c r="AU75" s="16">
         <f t="shared" si="167"/>
         <v>0.14851006001488046</v>
       </c>
-      <c r="AV75" s="17"/>
-      <c r="AW75" s="17"/>
-      <c r="AX75" s="17"/>
+      <c r="AV75" s="16"/>
+      <c r="AW75" s="16"/>
+      <c r="AX75" s="16"/>
     </row>
     <row r="76" spans="2:109" x14ac:dyDescent="0.2">
-      <c r="B76" s="19" t="s">
+      <c r="B76" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C76" s="17"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="17"/>
-      <c r="G76" s="17">
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="16">
         <f t="shared" ref="G76:K76" si="168">+G59/G51</f>
         <v>0.1246421493063202</v>
       </c>
-      <c r="H76" s="17">
+      <c r="H76" s="16">
         <f t="shared" si="168"/>
         <v>0.14503937007874015</v>
       </c>
-      <c r="I76" s="17">
+      <c r="I76" s="16">
         <f t="shared" si="168"/>
         <v>0.18895763921941933</v>
       </c>
-      <c r="J76" s="17">
+      <c r="J76" s="16">
         <f t="shared" si="168"/>
         <v>0.18838028169014084</v>
       </c>
-      <c r="K76" s="17">
+      <c r="K76" s="16">
         <f t="shared" si="168"/>
         <v>0.20618212197159566</v>
       </c>
-      <c r="L76" s="17">
+      <c r="L76" s="16">
         <f t="shared" ref="L76" si="169">+L59/L51</f>
         <v>0.20990722332670642</v>
       </c>
-      <c r="M76" s="17">
+      <c r="M76" s="16">
         <f t="shared" ref="M76" si="170">+M59/M51</f>
         <v>0.23520693193478509</v>
       </c>
-      <c r="N76" s="17">
+      <c r="N76" s="16">
         <f>+N59/N51</f>
         <v>0.19229337304542071</v>
       </c>
-      <c r="O76" s="17">
+      <c r="O76" s="16">
         <f t="shared" ref="O76:AD76" si="171">+O59/O51</f>
         <v>0.21320627586870727</v>
       </c>
-      <c r="P76" s="17">
+      <c r="P76" s="16">
         <f t="shared" si="171"/>
         <v>0.24117745442381669</v>
       </c>
-      <c r="Q76" s="17">
+      <c r="Q76" s="16">
         <f t="shared" si="171"/>
         <v>0.26604637639020134</v>
       </c>
-      <c r="R76" s="17">
+      <c r="R76" s="16">
         <f t="shared" si="171"/>
         <v>0.27354816863254133</v>
       </c>
-      <c r="S76" s="17">
+      <c r="S76" s="16">
         <f t="shared" si="171"/>
         <v>0.29110684580934099</v>
       </c>
-      <c r="T76" s="17">
+      <c r="T76" s="16">
         <f t="shared" si="171"/>
         <v>0.24997047360340144</v>
       </c>
-      <c r="U76" s="17">
+      <c r="U76" s="16">
         <f t="shared" si="171"/>
         <v>0.25086231005873033</v>
       </c>
-      <c r="V76" s="17">
+      <c r="V76" s="16">
         <f t="shared" si="171"/>
         <v>0.25257794296679104</v>
       </c>
-      <c r="W76" s="17">
+      <c r="W76" s="16">
         <f t="shared" si="171"/>
         <v>0.19336448197522396</v>
       </c>
-      <c r="X76" s="17">
+      <c r="X76" s="16">
         <f t="shared" si="171"/>
         <v>0.18185100493440848</v>
       </c>
-      <c r="Y76" s="17">
+      <c r="Y76" s="16">
         <f t="shared" si="171"/>
         <v>0.17892933618843684</v>
       </c>
-      <c r="Z76" s="17">
+      <c r="Z76" s="16">
         <f t="shared" si="171"/>
         <v>0.17634203520483172</v>
       </c>
-      <c r="AA76" s="17">
+      <c r="AA76" s="16">
         <f t="shared" si="171"/>
         <v>0.1735129806112389</v>
       </c>
-      <c r="AB76" s="41">
+      <c r="AB76" s="40">
         <f t="shared" si="171"/>
         <v>0.17952941176470588</v>
       </c>
-      <c r="AC76" s="17">
+      <c r="AC76" s="16">
         <f t="shared" si="171"/>
         <v>0.15717279857679209</v>
       </c>
-      <c r="AD76" s="17">
+      <c r="AD76" s="16">
         <f t="shared" si="171"/>
         <v>0.15511900037130005</v>
       </c>
-      <c r="AE76" s="17">
-        <f t="shared" ref="AE76" si="172">+AE59/AE51</f>
+      <c r="AE76" s="16">
+        <f t="shared" ref="AE76:AF76" si="172">+AE59/AE51</f>
         <v>0.16307214895267649</v>
       </c>
-      <c r="AF76" s="17"/>
-      <c r="AG76" s="17"/>
-      <c r="AH76" s="17"/>
-      <c r="AQ76" s="17">
+      <c r="AF76" s="16">
+        <f t="shared" si="172"/>
+        <v>0.17238620199146515</v>
+      </c>
+      <c r="AG76" s="16"/>
+      <c r="AH76" s="16"/>
+      <c r="AQ76" s="16">
         <f t="shared" ref="AQ76:BF76" si="173">+AQ59/AQ51</f>
         <v>0</v>
       </c>
-      <c r="AR76" s="17">
+      <c r="AR76" s="16">
         <f t="shared" si="173"/>
         <v>0</v>
       </c>
-      <c r="AS76" s="17">
+      <c r="AS76" s="16">
         <f t="shared" si="173"/>
         <v>0.25</v>
       </c>
-      <c r="AT76" s="17">
+      <c r="AT76" s="16">
         <f t="shared" si="173"/>
         <v>0.18248891736331416</v>
       </c>
-      <c r="AU76" s="17">
+      <c r="AU76" s="16">
         <f t="shared" si="173"/>
         <v>0.16471225777031828</v>
       </c>
-      <c r="AV76" s="17">
+      <c r="AV76" s="16">
         <f t="shared" si="173"/>
         <v>0.22985752587485617</v>
       </c>
-      <c r="AW76" s="17">
+      <c r="AW76" s="16">
         <f t="shared" si="173"/>
         <v>0.25506572778682646</v>
       </c>
-      <c r="AX76" s="17">
+      <c r="AX76" s="16">
         <f t="shared" si="173"/>
         <v>0.25239469462195546</v>
       </c>
-      <c r="AY76" s="17">
+      <c r="AY76" s="16">
         <f t="shared" si="173"/>
         <v>0.2688449395488649</v>
       </c>
-      <c r="AZ76" s="17">
+      <c r="AZ76" s="16">
         <f t="shared" si="173"/>
         <v>0.28443112518959862</v>
       </c>
-      <c r="BA76" s="17">
+      <c r="BA76" s="16">
         <f t="shared" si="173"/>
         <v>0.2993291081869508</v>
       </c>
-      <c r="BB76" s="17">
+      <c r="BB76" s="16">
         <f t="shared" si="173"/>
         <v>0.29953516962407462</v>
       </c>
-      <c r="BC76" s="17">
+      <c r="BC76" s="16">
         <f t="shared" si="173"/>
         <v>0.29968042854680105</v>
       </c>
-      <c r="BD76" s="17">
+      <c r="BD76" s="16">
         <f t="shared" si="173"/>
         <v>0.2997689777818105</v>
       </c>
-      <c r="BE76" s="17">
+      <c r="BE76" s="16">
         <f t="shared" si="173"/>
         <v>0.29980465126954314</v>
       </c>
-      <c r="BF76" s="17">
+      <c r="BF76" s="16">
         <f t="shared" si="173"/>
         <v>0.29979104278173424</v>
       </c>
     </row>
     <row r="77" spans="2:109" x14ac:dyDescent="0.2">
-      <c r="B77" s="15"/>
-      <c r="R77" s="17"/>
-      <c r="S77" s="17"/>
-      <c r="T77" s="17"/>
-      <c r="U77" s="17"/>
-      <c r="V77" s="17"/>
-      <c r="W77" s="17"/>
-      <c r="X77" s="17"/>
-      <c r="Y77" s="17"/>
-      <c r="Z77" s="17"/>
-      <c r="AA77" s="17"/>
-      <c r="AB77" s="17"/>
-      <c r="AC77" s="17"/>
-      <c r="AD77" s="17"/>
-      <c r="AE77" s="17"/>
-      <c r="AF77" s="17"/>
-      <c r="AG77" s="17"/>
-      <c r="AH77" s="17"/>
+      <c r="B77" s="14"/>
+      <c r="R77" s="16"/>
+      <c r="S77" s="16"/>
+      <c r="T77" s="16"/>
+      <c r="U77" s="16"/>
+      <c r="V77" s="16"/>
+      <c r="W77" s="16"/>
+      <c r="X77" s="16"/>
+      <c r="Y77" s="16"/>
+      <c r="Z77" s="16"/>
+      <c r="AA77" s="16"/>
+      <c r="AB77" s="16"/>
+      <c r="AC77" s="16"/>
+      <c r="AD77" s="16"/>
+      <c r="AE77" s="16"/>
+      <c r="AF77" s="16"/>
+      <c r="AG77" s="16"/>
+      <c r="AH77" s="16"/>
     </row>
     <row r="78" spans="2:109" x14ac:dyDescent="0.2">
-      <c r="BG78" s="28" t="s">
+      <c r="BG78" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="BH78" s="26">
+      <c r="BH78" s="25">
         <v>-0.01</v>
       </c>
     </row>
@@ -8561,10 +8676,10 @@
       <c r="AF79" s="5"/>
       <c r="AG79" s="5"/>
       <c r="AH79" s="5"/>
-      <c r="BG79" s="28" t="s">
+      <c r="BG79" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="BH79" s="30">
+      <c r="BH79" s="29">
         <v>0.08</v>
       </c>
     </row>
@@ -8633,12 +8748,12 @@
       <c r="AF80" s="5"/>
       <c r="AG80" s="5"/>
       <c r="AH80" s="5"/>
-      <c r="BG80" s="28" t="s">
+      <c r="BG80" s="27" t="s">
         <v>111</v>
       </c>
       <c r="BH80" s="4">
         <f>NPV(BH79,AV67:DF67)+Main!K5-Main!K6</f>
-        <v>1187377.0517001939</v>
+        <v>1187472.0517001939</v>
       </c>
     </row>
     <row r="81" spans="2:60" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -8706,10 +8821,10 @@
       <c r="AF81" s="5"/>
       <c r="AG81" s="5"/>
       <c r="AH81" s="5"/>
-      <c r="BG81" s="28" t="s">
+      <c r="BG81" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="BH81" s="26">
+      <c r="BH81" s="25">
         <v>0.1</v>
       </c>
     </row>
@@ -8778,12 +8893,12 @@
       <c r="AF82" s="5"/>
       <c r="AG82" s="5"/>
       <c r="AH82" s="5"/>
-      <c r="BG82" s="28" t="s">
+      <c r="BG82" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="BH82" s="20">
+      <c r="BH82" s="19">
         <f>BH80/Main!K3</f>
-        <v>368.64116551635846</v>
+        <v>368.15714418849501</v>
       </c>
     </row>
     <row r="83" spans="2:60" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -8944,7 +9059,7 @@
       <c r="AH85" s="5"/>
     </row>
     <row r="86" spans="2:60" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B86" s="18" t="s">
+      <c r="B86" s="17" t="s">
         <v>68</v>
       </c>
       <c r="C86" s="5"/>
@@ -9462,7 +9577,7 @@
       <c r="AH93" s="5"/>
     </row>
     <row r="94" spans="2:60" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B94" s="29" t="s">
+      <c r="B94" s="28" t="s">
         <v>114</v>
       </c>
       <c r="C94" s="5"/>
@@ -9613,7 +9728,7 @@
         <f t="shared" ref="Y95" si="190">X95+Y67</f>
         <v>26958</v>
       </c>
-      <c r="Z95" s="36">
+      <c r="Z95" s="35">
         <f>16398+12696</f>
         <v>29094</v>
       </c>
@@ -10474,7 +10589,7 @@
       <c r="S116" s="5"/>
     </row>
     <row r="117" spans="2:58" x14ac:dyDescent="0.2">
-      <c r="B117" s="33" t="s">
+      <c r="B117" s="32" t="s">
         <v>154</v>
       </c>
       <c r="S117" s="5"/>
@@ -10493,7 +10608,7 @@
       </c>
     </row>
     <row r="118" spans="2:58" x14ac:dyDescent="0.2">
-      <c r="B118" s="33" t="s">
+      <c r="B118" s="32" t="s">
         <v>160</v>
       </c>
       <c r="S118" s="5"/>
@@ -10556,7 +10671,7 @@
       </c>
     </row>
     <row r="119" spans="2:58" x14ac:dyDescent="0.2">
-      <c r="B119" s="33" t="s">
+      <c r="B119" s="32" t="s">
         <v>161</v>
       </c>
       <c r="S119" s="5"/>
@@ -10571,7 +10686,7 @@
       </c>
     </row>
     <row r="120" spans="2:58" x14ac:dyDescent="0.2">
-      <c r="B120" s="33"/>
+      <c r="B120" s="32"/>
       <c r="S120" s="5"/>
       <c r="Z120" s="5"/>
       <c r="AA120" s="5"/>
@@ -10580,7 +10695,7 @@
       <c r="AT120" s="4"/>
     </row>
     <row r="121" spans="2:58" x14ac:dyDescent="0.2">
-      <c r="B121" s="33" t="s">
+      <c r="B121" s="32" t="s">
         <v>162</v>
       </c>
       <c r="S121" s="5"/>
@@ -10642,58 +10757,58 @@
       </c>
     </row>
     <row r="122" spans="2:58" x14ac:dyDescent="0.2">
-      <c r="B122" s="33" t="s">
+      <c r="B122" s="32" t="s">
         <v>163</v>
       </c>
       <c r="S122" s="5"/>
-      <c r="AT122" s="26">
+      <c r="AT122" s="25">
         <f>+AT117/AS117-1</f>
         <v>0.21386886371438374</v>
       </c>
     </row>
     <row r="123" spans="2:58" x14ac:dyDescent="0.2">
-      <c r="B123" s="33" t="s">
+      <c r="B123" s="32" t="s">
         <v>164</v>
       </c>
       <c r="S123" s="5"/>
-      <c r="AT123" s="26">
+      <c r="AT123" s="25">
         <f>+AT121*1000/AT37</f>
         <v>8.3007064654555152E-2</v>
       </c>
-      <c r="AU123" s="26">
+      <c r="AU123" s="25">
         <v>0.12</v>
       </c>
-      <c r="AV123" s="26">
+      <c r="AV123" s="25">
         <v>0.16</v>
       </c>
-      <c r="AW123" s="26">
+      <c r="AW123" s="25">
         <v>0.2</v>
       </c>
-      <c r="AX123" s="26">
+      <c r="AX123" s="25">
         <v>0.24</v>
       </c>
-      <c r="AY123" s="26">
+      <c r="AY123" s="25">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AZ123" s="26">
+      <c r="AZ123" s="25">
         <v>0.32</v>
       </c>
-      <c r="BA123" s="26">
+      <c r="BA123" s="25">
         <v>0.36</v>
       </c>
-      <c r="BB123" s="26">
+      <c r="BB123" s="25">
         <v>0.37</v>
       </c>
-      <c r="BC123" s="26">
+      <c r="BC123" s="25">
         <v>0.38</v>
       </c>
-      <c r="BD123" s="26">
+      <c r="BD123" s="25">
         <v>0.39</v>
       </c>
-      <c r="BE123" s="26">
+      <c r="BE123" s="25">
         <v>0.4</v>
       </c>
-      <c r="BF123" s="26">
+      <c r="BF123" s="25">
         <v>0.41</v>
       </c>
     </row>
@@ -10718,120 +10833,120 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="28"/>
-    <col min="3" max="3" width="11.7109375" style="28" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="28"/>
+    <col min="1" max="1" width="5" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="27"/>
+    <col min="3" max="3" width="11.7109375" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="27">
         <v>100000</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="27">
         <v>550000</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="27">
         <v>750000</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="27">
         <v>950000</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="27">
         <v>350000</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="27">
         <v>375000</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="27">
         <v>250000</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="27">
         <v>300000</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="27">
         <v>125000</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="27">
         <v>300000</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="27">
         <v>300000</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="27">
         <v>300000</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="32" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="32" t="s">
         <v>158</v>
       </c>
     </row>
@@ -10853,12 +10968,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5" style="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="33"/>
+    <col min="1" max="1" width="5" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>